<commit_message>
Apply some review comments
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/sendDashboard/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/sendDashboard/TestData.xlsx
@@ -12,15 +12,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="102">
   <si>
     <t>Supported Browser Types</t>
   </si>
   <si>
+    <t>Variable</t>
+  </si>
+  <si>
     <t>MozillaFirefox</t>
   </si>
   <si>
-    <t>Variable</t>
+    <t>GoogleChrome</t>
+  </si>
+  <si>
+    <t>MicrosoftInternetExplorer</t>
+  </si>
+  <si>
+    <t>MicrosoftEdge</t>
   </si>
   <si>
     <t>Data1</t>
@@ -38,15 +47,6 @@
     <t>URLs</t>
   </si>
   <si>
-    <t>GoogleChrome</t>
-  </si>
-  <si>
-    <t>MicrosoftInternetExplorer</t>
-  </si>
-  <si>
-    <t>MicrosoftEdge</t>
-  </si>
-  <si>
     <t>URL_login_login</t>
   </si>
   <si>
@@ -312,6 +312,12 @@
   </si>
   <si>
     <t>Sending Dashboard</t>
+  </si>
+  <si>
+    <t>HideNotificationToolTipText</t>
+  </si>
+  <si>
+    <t>Incorta email notifications are sent with auto-generated text that contains the sender name, the dashboard name, and for CSV/XLSX formats, the filters applied to the dashboard. Toggle this option on to hide this text.</t>
   </si>
 </sst>
 </file>
@@ -455,19 +461,19 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -482,7 +488,7 @@
     </row>
     <row r="2" ht="13.5" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="5"/>
@@ -1479,7 +1485,14 @@
         <v>99</v>
       </c>
     </row>
-    <row r="50" ht="15.75" customHeight="1"/>
+    <row r="50" ht="15.75" customHeight="1">
+      <c r="A50" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>101</v>
+      </c>
+    </row>
     <row r="51" ht="15.75" customHeight="1"/>
     <row r="52" ht="15.75" customHeight="1"/>
     <row r="53" ht="15.75" customHeight="1"/>
@@ -2486,7 +2499,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2501,7 +2514,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -2516,7 +2529,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -2531,7 +2544,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>

</xml_diff>

<commit_message>
TCs in SendDashboardTest.java is updated with new functions created in AllContent_Dashboard.java.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/sendDashboard/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/sendDashboard/TestData.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="107">
   <si>
     <t>Supported Browser Types</t>
   </si>
@@ -318,6 +318,21 @@
   </si>
   <si>
     <t>Incorta email notifications are sent with auto-generated text that contains the sender name, the dashboard name, and for CSV/XLSX formats, the filters applied to the dashboard. Toggle this option on to hide this text.</t>
+  </si>
+  <si>
+    <t>html</t>
+  </si>
+  <si>
+    <t>The dashboard will be sent in the same layout it appears now. Insights can be downloaded as images.</t>
+  </si>
+  <si>
+    <t>xlsx</t>
+  </si>
+  <si>
+    <t>An XLSX file will be sent only for the tables and pivot tables in the dashboard.</t>
+  </si>
+  <si>
+    <t>A CSV file will be sent only for the first table in this dashboard.</t>
   </si>
 </sst>
 </file>
@@ -1493,9 +1508,30 @@
         <v>101</v>
       </c>
     </row>
-    <row r="51" ht="15.75" customHeight="1"/>
-    <row r="52" ht="15.75" customHeight="1"/>
-    <row r="53" ht="15.75" customHeight="1"/>
+    <row r="51" ht="15.75" customHeight="1">
+      <c r="A51" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="52" ht="15.75" customHeight="1">
+      <c r="A52" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="53" ht="15.75" customHeight="1">
+      <c r="A53" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B53" s="10" t="s">
+        <v>106</v>
+      </c>
+    </row>
     <row r="54" ht="15.75" customHeight="1"/>
     <row r="55" ht="15.75" customHeight="1"/>
     <row r="56" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Added New functions in AllContantDashboard.java and new 6 TCs in new class SchedileDashboardTest.java and updated TestData.xlsx
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/sendDashboard/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/sendDashboard/TestData.xlsx
@@ -12,12 +12,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="114">
+  <si>
+    <t>Variable</t>
+  </si>
   <si>
     <t>Supported Browser Types</t>
   </si>
   <si>
-    <t>Variable</t>
+    <t>Data1</t>
+  </si>
+  <si>
+    <t>Data2</t>
+  </si>
+  <si>
+    <t>Data3</t>
+  </si>
+  <si>
+    <t>Data4</t>
+  </si>
+  <si>
+    <t>URLs</t>
   </si>
   <si>
     <t>MozillaFirefox</t>
@@ -32,21 +47,6 @@
     <t>MicrosoftEdge</t>
   </si>
   <si>
-    <t>Data1</t>
-  </si>
-  <si>
-    <t>Data2</t>
-  </si>
-  <si>
-    <t>Data3</t>
-  </si>
-  <si>
-    <t>Data4</t>
-  </si>
-  <si>
-    <t>URLs</t>
-  </si>
-  <si>
     <t>URL_login_login</t>
   </si>
   <si>
@@ -318,6 +318,42 @@
   </si>
   <si>
     <t>Incorta email notifications are sent with auto-generated text that contains the sender name, the dashboard name, and for CSV/XLSX formats, the filters applied to the dashboard. Toggle this option on to hide this text.</t>
+  </si>
+  <si>
+    <t>html</t>
+  </si>
+  <si>
+    <t>The dashboard will be sent in the same layout it appears now. Insights can be downloaded as images.</t>
+  </si>
+  <si>
+    <t>xlsx</t>
+  </si>
+  <si>
+    <t>An XLSX file will be sent only for the tables and pivot tables in the dashboard.</t>
+  </si>
+  <si>
+    <t>A CSV file will be sent only for the first table in this dashboard.</t>
+  </si>
+  <si>
+    <t>Schedule Dashboard via email</t>
+  </si>
+  <si>
+    <t>JobName</t>
+  </si>
+  <si>
+    <t>Duplicate Job Name</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Ahmed.Abdelsalam@incorta.com</t>
+  </si>
+  <si>
+    <t>DuplicateJobNameErrorMessage</t>
+  </si>
+  <si>
+    <t>INC_004010050:Another SCHEDULER with the same name [Duplicate Job Name] already exists.</t>
   </si>
 </sst>
 </file>
@@ -400,11 +436,11 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="2" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
@@ -460,35 +496,35 @@
   </cols>
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
-      <c r="A1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
     </row>
     <row r="2" ht="13.5" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="5"/>
@@ -1493,14 +1529,76 @@
         <v>101</v>
       </c>
     </row>
-    <row r="51" ht="15.75" customHeight="1"/>
-    <row r="52" ht="15.75" customHeight="1"/>
-    <row r="53" ht="15.75" customHeight="1"/>
-    <row r="54" ht="15.75" customHeight="1"/>
-    <row r="55" ht="15.75" customHeight="1"/>
-    <row r="56" ht="15.75" customHeight="1"/>
-    <row r="57" ht="15.75" customHeight="1"/>
-    <row r="58" ht="15.75" customHeight="1"/>
+    <row r="51" ht="15.75" customHeight="1">
+      <c r="A51" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="52" ht="15.75" customHeight="1">
+      <c r="A52" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="53" ht="15.75" customHeight="1">
+      <c r="A53" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B53" s="10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="54" ht="13.5" customHeight="1">
+      <c r="A54" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B54" s="4"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
+      <c r="H54" s="6"/>
+      <c r="I54" s="6"/>
+      <c r="J54" s="6"/>
+      <c r="K54" s="6"/>
+      <c r="L54" s="6"/>
+      <c r="M54" s="6"/>
+      <c r="N54" s="6"/>
+      <c r="O54" s="6"/>
+    </row>
+    <row r="55" ht="15.75" customHeight="1">
+      <c r="A55" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="56" ht="15.75" customHeight="1">
+      <c r="A56" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B56" s="10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="57" ht="15.75" customHeight="1">
+      <c r="A57" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B57" s="10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="58" ht="15.75" customHeight="1">
+      <c r="B58" s="10"/>
+    </row>
     <row r="59" ht="15.75" customHeight="1"/>
     <row r="60" ht="15.75" customHeight="1"/>
     <row r="61" ht="15.75" customHeight="1"/>
@@ -2444,11 +2542,12 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
     <mergeCell ref="A16:C16"/>
     <mergeCell ref="A18:C18"/>
     <mergeCell ref="A45:C45"/>
     <mergeCell ref="A48:C48"/>
+    <mergeCell ref="A54:C54"/>
     <mergeCell ref="A21:C21"/>
     <mergeCell ref="A27:C27"/>
     <mergeCell ref="A35:C35"/>
@@ -2483,79 +2582,79 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
+      <c r="A5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Added new TCs - Updated functions name - Added new functions.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/sendDashboard/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/sendDashboard/TestData.xlsx
@@ -12,29 +12,47 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="116">
   <si>
     <t>Variable</t>
   </si>
   <si>
+    <t>Data1</t>
+  </si>
+  <si>
+    <t>Data2</t>
+  </si>
+  <si>
+    <t>Data3</t>
+  </si>
+  <si>
+    <t>Data4</t>
+  </si>
+  <si>
+    <t>URLs</t>
+  </si>
+  <si>
+    <t>URL_login_login</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>URL_content_allContent</t>
+  </si>
+  <si>
+    <t>all-content/0</t>
+  </si>
+  <si>
+    <t>URL_security_groups</t>
+  </si>
+  <si>
+    <t>security/groups</t>
+  </si>
+  <si>
     <t>Supported Browser Types</t>
   </si>
   <si>
-    <t>Data1</t>
-  </si>
-  <si>
-    <t>Data2</t>
-  </si>
-  <si>
-    <t>Data3</t>
-  </si>
-  <si>
-    <t>Data4</t>
-  </si>
-  <si>
-    <t>URLs</t>
-  </si>
-  <si>
     <t>MozillaFirefox</t>
   </si>
   <si>
@@ -47,24 +65,6 @@
     <t>MicrosoftEdge</t>
   </si>
   <si>
-    <t>URL_login_login</t>
-  </si>
-  <si>
-    <t>login</t>
-  </si>
-  <si>
-    <t>URL_content_allContent</t>
-  </si>
-  <si>
-    <t>all-content/0</t>
-  </si>
-  <si>
-    <t>URL_security_groups</t>
-  </si>
-  <si>
-    <t>security/groups</t>
-  </si>
-  <si>
     <t>URL_security_users</t>
   </si>
   <si>
@@ -354,6 +354,12 @@
   </si>
   <si>
     <t>INC_004010050:Another SCHEDULER with the same name [Duplicate Job Name] already exists.</t>
+  </si>
+  <si>
+    <t>AppendTimeStampHelpText</t>
+  </si>
+  <si>
+    <t>File names are appended with a timestamp when they are generated. Toggling this option off will remove the timestamp. If you are sending this to a shared folder, the file will be overwritten.</t>
   </si>
 </sst>
 </file>
@@ -439,9 +445,6 @@
     <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
     <xf borderId="2" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -451,6 +454,9 @@
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -489,7 +495,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="27.86"/>
-    <col customWidth="1" min="2" max="2" width="64.29"/>
+    <col customWidth="1" min="2" max="2" width="180.71"/>
     <col customWidth="1" min="3" max="3" width="36.14"/>
     <col customWidth="1" min="4" max="15" width="8.57"/>
     <col customWidth="1" min="16" max="26" width="8.71"/>
@@ -500,16 +506,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -523,995 +529,995 @@
       <c r="O1" s="1"/>
     </row>
     <row r="2" ht="13.5" customHeight="1">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+    </row>
+    <row r="3" ht="13.5" customHeight="1">
+      <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-    </row>
-    <row r="3" ht="13.5" customHeight="1">
-      <c r="A3" s="7" t="s">
+      <c r="B3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+    </row>
+    <row r="4" ht="13.5" customHeight="1">
+      <c r="A4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+    </row>
+    <row r="5" ht="13.5" customHeight="1">
+      <c r="A5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-    </row>
-    <row r="4" ht="13.5" customHeight="1">
-      <c r="A4" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-    </row>
-    <row r="5" ht="13.5" customHeight="1">
-      <c r="A5" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
     </row>
     <row r="6" ht="13.5" customHeight="1">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
     </row>
     <row r="7" ht="13.5" customHeight="1">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
     </row>
     <row r="8" ht="13.5" customHeight="1">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
     </row>
     <row r="9" ht="13.5" customHeight="1">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
     </row>
     <row r="10" ht="13.5" customHeight="1">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
     </row>
     <row r="11" ht="13.5" customHeight="1">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
     </row>
     <row r="12" ht="13.5" customHeight="1">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
     </row>
     <row r="13" ht="13.5" customHeight="1">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
     </row>
     <row r="14" ht="13.5" customHeight="1">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
-      <c r="O14" s="7"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
     </row>
     <row r="15" ht="13.5" customHeight="1">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
     </row>
     <row r="16" ht="13.5" customHeight="1">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
-      <c r="N16" s="6"/>
-      <c r="O16" s="6"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
     </row>
     <row r="17" ht="13.5" customHeight="1">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="7"/>
-      <c r="O17" s="7"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
     </row>
     <row r="18" ht="13.5" customHeight="1">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
-      <c r="N18" s="6"/>
-      <c r="O18" s="6"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
     </row>
     <row r="19" ht="13.5" customHeight="1">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
-      <c r="N19" s="7"/>
-      <c r="O19" s="7"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
     </row>
     <row r="20" ht="13.5" customHeight="1">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
-      <c r="N20" s="7"/>
-      <c r="O20" s="7"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
     </row>
     <row r="21" ht="13.5" customHeight="1">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
-      <c r="N21" s="6"/>
-      <c r="O21" s="6"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
     </row>
     <row r="22" ht="13.5" customHeight="1">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
-      <c r="L22" s="7"/>
-      <c r="M22" s="7"/>
-      <c r="N22" s="7"/>
-      <c r="O22" s="7"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="6"/>
     </row>
     <row r="23" ht="13.5" customHeight="1">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7"/>
-      <c r="L23" s="7"/>
-      <c r="M23" s="7"/>
-      <c r="N23" s="7"/>
-      <c r="O23" s="7"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="6"/>
     </row>
     <row r="24" ht="13.5" customHeight="1">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="7"/>
-      <c r="M24" s="7"/>
-      <c r="N24" s="7"/>
-      <c r="O24" s="7"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
     </row>
     <row r="25" ht="13.5" customHeight="1">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="7">
+      <c r="B25" s="6">
         <v>30.0</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C25" s="6">
         <v>30.0</v>
       </c>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="7"/>
-      <c r="L25" s="7"/>
-      <c r="M25" s="7"/>
-      <c r="N25" s="7"/>
-      <c r="O25" s="7"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="6"/>
+      <c r="O25" s="6"/>
     </row>
     <row r="26" ht="13.5" customHeight="1">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C26" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
-      <c r="J26" s="7"/>
-      <c r="K26" s="7"/>
-      <c r="L26" s="7"/>
-      <c r="M26" s="7"/>
-      <c r="N26" s="7"/>
-      <c r="O26" s="7"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="6"/>
+      <c r="O26" s="6"/>
     </row>
     <row r="27" ht="13.5" customHeight="1">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="6"/>
-      <c r="K27" s="6"/>
-      <c r="L27" s="6"/>
-      <c r="M27" s="6"/>
-      <c r="N27" s="6"/>
-      <c r="O27" s="6"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="5"/>
     </row>
     <row r="28" ht="13.5" customHeight="1">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B28" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
-      <c r="J28" s="7"/>
-      <c r="K28" s="7"/>
-      <c r="L28" s="7"/>
-      <c r="M28" s="7"/>
-      <c r="N28" s="7"/>
-      <c r="O28" s="7"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="6"/>
+      <c r="M28" s="6"/>
+      <c r="N28" s="6"/>
+      <c r="O28" s="6"/>
     </row>
     <row r="29" ht="13.5" customHeight="1">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
-      <c r="J29" s="7"/>
-      <c r="K29" s="7"/>
-      <c r="L29" s="7"/>
-      <c r="M29" s="7"/>
-      <c r="N29" s="7"/>
-      <c r="O29" s="7"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="6"/>
+      <c r="M29" s="6"/>
+      <c r="N29" s="6"/>
+      <c r="O29" s="6"/>
     </row>
     <row r="30" ht="13.5" customHeight="1">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="B30" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
-      <c r="J30" s="7"/>
-      <c r="K30" s="7"/>
-      <c r="L30" s="7"/>
-      <c r="M30" s="7"/>
-      <c r="N30" s="7"/>
-      <c r="O30" s="7"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="6"/>
+      <c r="M30" s="6"/>
+      <c r="N30" s="6"/>
+      <c r="O30" s="6"/>
     </row>
     <row r="31" ht="13.5" customHeight="1">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="7"/>
-      <c r="K31" s="7"/>
-      <c r="L31" s="7"/>
-      <c r="M31" s="7"/>
-      <c r="N31" s="7"/>
-      <c r="O31" s="7"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="6"/>
+      <c r="M31" s="6"/>
+      <c r="N31" s="6"/>
+      <c r="O31" s="6"/>
     </row>
     <row r="32" ht="13.5" customHeight="1">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B32" s="4"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="6"/>
-      <c r="J32" s="6"/>
-      <c r="K32" s="6"/>
-      <c r="L32" s="6"/>
-      <c r="M32" s="6"/>
-      <c r="N32" s="6"/>
-      <c r="O32" s="6"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5"/>
+      <c r="M32" s="5"/>
+      <c r="N32" s="5"/>
+      <c r="O32" s="5"/>
     </row>
     <row r="33" ht="13.5" customHeight="1">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C33" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
-      <c r="J33" s="7"/>
-      <c r="K33" s="7"/>
-      <c r="L33" s="7"/>
-      <c r="M33" s="7"/>
-      <c r="N33" s="7"/>
-      <c r="O33" s="7"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
+      <c r="L33" s="6"/>
+      <c r="M33" s="6"/>
+      <c r="N33" s="6"/>
+      <c r="O33" s="6"/>
     </row>
     <row r="34" ht="13.5" customHeight="1">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C34" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="7"/>
-      <c r="I34" s="7"/>
-      <c r="J34" s="7"/>
-      <c r="K34" s="7"/>
-      <c r="L34" s="7"/>
-      <c r="M34" s="7"/>
-      <c r="N34" s="7"/>
-      <c r="O34" s="7"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+      <c r="K34" s="6"/>
+      <c r="L34" s="6"/>
+      <c r="M34" s="6"/>
+      <c r="N34" s="6"/>
+      <c r="O34" s="6"/>
     </row>
     <row r="35" ht="13.5" customHeight="1">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B35" s="4"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6"/>
-      <c r="I35" s="6"/>
-      <c r="J35" s="6"/>
-      <c r="K35" s="6"/>
-      <c r="L35" s="6"/>
-      <c r="M35" s="6"/>
-      <c r="N35" s="6"/>
-      <c r="O35" s="6"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="5"/>
+      <c r="M35" s="5"/>
+      <c r="N35" s="5"/>
+      <c r="O35" s="5"/>
     </row>
     <row r="36" ht="13.5" customHeight="1">
-      <c r="A36" s="7" t="s">
+      <c r="A36" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="7"/>
-      <c r="H36" s="7"/>
-      <c r="I36" s="7"/>
-      <c r="J36" s="7"/>
-      <c r="K36" s="7"/>
-      <c r="L36" s="7"/>
-      <c r="M36" s="7"/>
-      <c r="N36" s="7"/>
-      <c r="O36" s="7"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="6"/>
+      <c r="K36" s="6"/>
+      <c r="L36" s="6"/>
+      <c r="M36" s="6"/>
+      <c r="N36" s="6"/>
+      <c r="O36" s="6"/>
     </row>
     <row r="37" ht="13.5" customHeight="1">
-      <c r="A37" s="7" t="s">
+      <c r="A37" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="B37" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7"/>
-      <c r="H37" s="7"/>
-      <c r="I37" s="7"/>
-      <c r="J37" s="7"/>
-      <c r="K37" s="7"/>
-      <c r="L37" s="7"/>
-      <c r="M37" s="7"/>
-      <c r="N37" s="7"/>
-      <c r="O37" s="7"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="6"/>
+      <c r="K37" s="6"/>
+      <c r="L37" s="6"/>
+      <c r="M37" s="6"/>
+      <c r="N37" s="6"/>
+      <c r="O37" s="6"/>
     </row>
     <row r="38" ht="13.5" customHeight="1">
-      <c r="A38" s="7" t="s">
+      <c r="A38" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="B38" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="7"/>
-      <c r="I38" s="7"/>
-      <c r="J38" s="7"/>
-      <c r="K38" s="7"/>
-      <c r="L38" s="7"/>
-      <c r="M38" s="7"/>
-      <c r="N38" s="7"/>
-      <c r="O38" s="7"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="6"/>
+      <c r="K38" s="6"/>
+      <c r="L38" s="6"/>
+      <c r="M38" s="6"/>
+      <c r="N38" s="6"/>
+      <c r="O38" s="6"/>
     </row>
     <row r="39" ht="13.5" customHeight="1">
-      <c r="A39" s="7" t="s">
+      <c r="A39" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B39" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="7"/>
-      <c r="I39" s="7"/>
-      <c r="J39" s="7"/>
-      <c r="K39" s="7"/>
-      <c r="L39" s="7"/>
-      <c r="M39" s="7"/>
-      <c r="N39" s="7"/>
-      <c r="O39" s="7"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="6"/>
+      <c r="J39" s="6"/>
+      <c r="K39" s="6"/>
+      <c r="L39" s="6"/>
+      <c r="M39" s="6"/>
+      <c r="N39" s="6"/>
+      <c r="O39" s="6"/>
     </row>
     <row r="40" ht="13.5" customHeight="1">
-      <c r="A40" s="7" t="s">
+      <c r="A40" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B40" s="7" t="s">
+      <c r="B40" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="7"/>
-      <c r="I40" s="7"/>
-      <c r="J40" s="7"/>
-      <c r="K40" s="7"/>
-      <c r="L40" s="7"/>
-      <c r="M40" s="7"/>
-      <c r="N40" s="7"/>
-      <c r="O40" s="7"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="6"/>
+      <c r="J40" s="6"/>
+      <c r="K40" s="6"/>
+      <c r="L40" s="6"/>
+      <c r="M40" s="6"/>
+      <c r="N40" s="6"/>
+      <c r="O40" s="6"/>
     </row>
     <row r="41" ht="13.5" customHeight="1">
-      <c r="A41" s="7" t="s">
+      <c r="A41" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="B41" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="C41" s="7"/>
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="7"/>
-      <c r="H41" s="7"/>
-      <c r="I41" s="7"/>
-      <c r="J41" s="7"/>
-      <c r="K41" s="7"/>
-      <c r="L41" s="7"/>
-      <c r="M41" s="7"/>
-      <c r="N41" s="7"/>
-      <c r="O41" s="7"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
+      <c r="I41" s="6"/>
+      <c r="J41" s="6"/>
+      <c r="K41" s="6"/>
+      <c r="L41" s="6"/>
+      <c r="M41" s="6"/>
+      <c r="N41" s="6"/>
+      <c r="O41" s="6"/>
     </row>
     <row r="42" ht="13.5" customHeight="1">
-      <c r="A42" s="3" t="s">
+      <c r="A42" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B42" s="4"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6"/>
-      <c r="H42" s="6"/>
-      <c r="I42" s="6"/>
-      <c r="J42" s="6"/>
-      <c r="K42" s="6"/>
-      <c r="L42" s="6"/>
-      <c r="M42" s="6"/>
-      <c r="N42" s="6"/>
-      <c r="O42" s="6"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
+      <c r="I42" s="5"/>
+      <c r="J42" s="5"/>
+      <c r="K42" s="5"/>
+      <c r="L42" s="5"/>
+      <c r="M42" s="5"/>
+      <c r="N42" s="5"/>
+      <c r="O42" s="5"/>
     </row>
     <row r="43" ht="13.5" customHeight="1">
-      <c r="A43" s="7" t="s">
+      <c r="A43" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="B43" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="C43" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="D43" s="7" t="s">
+      <c r="D43" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="E43" s="7" t="s">
+      <c r="E43" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="F43" s="7"/>
-      <c r="G43" s="7"/>
-      <c r="H43" s="7"/>
-      <c r="I43" s="7"/>
-      <c r="J43" s="7"/>
-      <c r="K43" s="7"/>
-      <c r="L43" s="7"/>
-      <c r="M43" s="7"/>
-      <c r="N43" s="7"/>
-      <c r="O43" s="7"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="6"/>
+      <c r="J43" s="6"/>
+      <c r="K43" s="6"/>
+      <c r="L43" s="6"/>
+      <c r="M43" s="6"/>
+      <c r="N43" s="6"/>
+      <c r="O43" s="6"/>
     </row>
     <row r="44" ht="13.5" customHeight="1">
-      <c r="A44" s="7" t="s">
+      <c r="A44" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="B44" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="C44" s="7" t="s">
+      <c r="C44" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="D44" s="7" t="s">
+      <c r="D44" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="E44" s="7" t="s">
+      <c r="E44" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="F44" s="7"/>
-      <c r="G44" s="7"/>
-      <c r="H44" s="7"/>
-      <c r="I44" s="7"/>
-      <c r="J44" s="7"/>
-      <c r="K44" s="7"/>
-      <c r="L44" s="7"/>
-      <c r="M44" s="7"/>
-      <c r="N44" s="7"/>
-      <c r="O44" s="7"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="6"/>
+      <c r="I44" s="6"/>
+      <c r="J44" s="6"/>
+      <c r="K44" s="6"/>
+      <c r="L44" s="6"/>
+      <c r="M44" s="6"/>
+      <c r="N44" s="6"/>
+      <c r="O44" s="6"/>
     </row>
     <row r="45" ht="13.5" customHeight="1">
-      <c r="A45" s="3" t="s">
+      <c r="A45" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B45" s="4"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="6"/>
-      <c r="G45" s="6"/>
-      <c r="H45" s="6"/>
-      <c r="I45" s="6"/>
-      <c r="J45" s="6"/>
-      <c r="K45" s="6"/>
-      <c r="L45" s="6"/>
-      <c r="M45" s="6"/>
-      <c r="N45" s="6"/>
-      <c r="O45" s="6"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
+      <c r="J45" s="5"/>
+      <c r="K45" s="5"/>
+      <c r="L45" s="5"/>
+      <c r="M45" s="5"/>
+      <c r="N45" s="5"/>
+      <c r="O45" s="5"/>
     </row>
     <row r="46" ht="13.5" customHeight="1">
-      <c r="A46" s="7" t="s">
+      <c r="A46" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="B46" s="7" t="s">
+      <c r="B46" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="C46" s="7"/>
-      <c r="D46" s="7"/>
-      <c r="E46" s="7"/>
-      <c r="F46" s="7"/>
-      <c r="G46" s="7"/>
-      <c r="H46" s="7"/>
-      <c r="I46" s="7"/>
-      <c r="J46" s="7"/>
-      <c r="K46" s="7"/>
-      <c r="L46" s="7"/>
-      <c r="M46" s="7"/>
-      <c r="N46" s="7"/>
-      <c r="O46" s="7"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="6"/>
+      <c r="I46" s="6"/>
+      <c r="J46" s="6"/>
+      <c r="K46" s="6"/>
+      <c r="L46" s="6"/>
+      <c r="M46" s="6"/>
+      <c r="N46" s="6"/>
+      <c r="O46" s="6"/>
     </row>
     <row r="47" ht="13.5" customHeight="1">
-      <c r="A47" s="7" t="s">
+      <c r="A47" s="6" t="s">
         <v>95</v>
       </c>
       <c r="B47" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="C47" s="7"/>
-      <c r="D47" s="7"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="7"/>
-      <c r="G47" s="7"/>
-      <c r="H47" s="7"/>
-      <c r="I47" s="7"/>
-      <c r="J47" s="7"/>
-      <c r="K47" s="7"/>
-      <c r="L47" s="7"/>
-      <c r="M47" s="7"/>
-      <c r="N47" s="7"/>
-      <c r="O47" s="7"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
+      <c r="I47" s="6"/>
+      <c r="J47" s="6"/>
+      <c r="K47" s="6"/>
+      <c r="L47" s="6"/>
+      <c r="M47" s="6"/>
+      <c r="N47" s="6"/>
+      <c r="O47" s="6"/>
     </row>
     <row r="48" ht="13.5" customHeight="1">
       <c r="A48" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="B48" s="4"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="6"/>
-      <c r="F48" s="6"/>
-      <c r="G48" s="6"/>
-      <c r="H48" s="6"/>
-      <c r="I48" s="6"/>
-      <c r="J48" s="6"/>
-      <c r="K48" s="6"/>
-      <c r="L48" s="6"/>
-      <c r="M48" s="6"/>
-      <c r="N48" s="6"/>
-      <c r="O48" s="6"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5"/>
+      <c r="I48" s="5"/>
+      <c r="J48" s="5"/>
+      <c r="K48" s="5"/>
+      <c r="L48" s="5"/>
+      <c r="M48" s="5"/>
+      <c r="N48" s="5"/>
+      <c r="O48" s="5"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="10" t="s">
@@ -1557,20 +1563,20 @@
       <c r="A54" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="B54" s="4"/>
-      <c r="C54" s="5"/>
-      <c r="D54" s="6"/>
-      <c r="E54" s="6"/>
-      <c r="F54" s="6"/>
-      <c r="G54" s="6"/>
-      <c r="H54" s="6"/>
-      <c r="I54" s="6"/>
-      <c r="J54" s="6"/>
-      <c r="K54" s="6"/>
-      <c r="L54" s="6"/>
-      <c r="M54" s="6"/>
-      <c r="N54" s="6"/>
-      <c r="O54" s="6"/>
+      <c r="B54" s="3"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="5"/>
+      <c r="I54" s="5"/>
+      <c r="J54" s="5"/>
+      <c r="K54" s="5"/>
+      <c r="L54" s="5"/>
+      <c r="M54" s="5"/>
+      <c r="N54" s="5"/>
+      <c r="O54" s="5"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
       <c r="A55" s="10" t="s">
@@ -1597,7 +1603,12 @@
       </c>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="B58" s="10"/>
+      <c r="A58" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="59" ht="15.75" customHeight="1"/>
     <row r="60" ht="15.75" customHeight="1"/>
@@ -2582,79 +2593,79 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
+      <c r="A1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
+      <c r="A2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
+      <c r="A3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
+      <c r="A4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
+      <c r="A5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Added new temp class for creating 200 jobs. Added new functions and TCs.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/sendDashboard/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/sendDashboard/TestData.xlsx
@@ -12,11 +12,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="127">
   <si>
     <t>Variable</t>
   </si>
   <si>
+    <t>Supported Browser Types</t>
+  </si>
+  <si>
     <t>Data1</t>
   </si>
   <si>
@@ -32,6 +35,18 @@
     <t>URLs</t>
   </si>
   <si>
+    <t>MozillaFirefox</t>
+  </si>
+  <si>
+    <t>GoogleChrome</t>
+  </si>
+  <si>
+    <t>MicrosoftInternetExplorer</t>
+  </si>
+  <si>
+    <t>MicrosoftEdge</t>
+  </si>
+  <si>
     <t>URL_login_login</t>
   </si>
   <si>
@@ -50,21 +65,6 @@
     <t>security/groups</t>
   </si>
   <si>
-    <t>Supported Browser Types</t>
-  </si>
-  <si>
-    <t>MozillaFirefox</t>
-  </si>
-  <si>
-    <t>GoogleChrome</t>
-  </si>
-  <si>
-    <t>MicrosoftInternetExplorer</t>
-  </si>
-  <si>
-    <t>MicrosoftEdge</t>
-  </si>
-  <si>
     <t>URL_security_users</t>
   </si>
   <si>
@@ -360,6 +360,39 @@
   </si>
   <si>
     <t>File names are appended with a timestamp when they are generated. Toggling this option off will remove the timestamp. If you are sending this to a shared folder, the file will be overwritten.</t>
+  </si>
+  <si>
+    <t>ScheduleJobName</t>
+  </si>
+  <si>
+    <t>UpdateJob</t>
+  </si>
+  <si>
+    <t>ScheduleJobDescription</t>
+  </si>
+  <si>
+    <t>Automation_Job_Name</t>
+  </si>
+  <si>
+    <t>ScheduleJobDate</t>
+  </si>
+  <si>
+    <t>10/31/2021</t>
+  </si>
+  <si>
+    <t>ScheduleJobTime</t>
+  </si>
+  <si>
+    <t>03:30 PM</t>
+  </si>
+  <si>
+    <t>ScheduleJobTimeZone</t>
+  </si>
+  <si>
+    <t>GMT+03:00</t>
+  </si>
+  <si>
+    <t>ScheduleJobRecurrence</t>
   </si>
 </sst>
 </file>
@@ -438,12 +471,15 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="2" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
@@ -456,9 +492,6 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -467,6 +500,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -506,16 +542,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -529,995 +565,995 @@
       <c r="O1" s="1"/>
     </row>
     <row r="2" ht="13.5" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
     </row>
     <row r="3" ht="13.5" customHeight="1">
-      <c r="A3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
+      <c r="A3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
     </row>
     <row r="4" ht="13.5" customHeight="1">
-      <c r="A4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
+      <c r="A4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
     </row>
     <row r="5" ht="13.5" customHeight="1">
-      <c r="A5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
+      <c r="A5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
     </row>
     <row r="6" ht="13.5" customHeight="1">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
     </row>
     <row r="7" ht="13.5" customHeight="1">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
     </row>
     <row r="8" ht="13.5" customHeight="1">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
     </row>
     <row r="9" ht="13.5" customHeight="1">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
     </row>
     <row r="10" ht="13.5" customHeight="1">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
     </row>
     <row r="11" ht="13.5" customHeight="1">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
     </row>
     <row r="12" ht="13.5" customHeight="1">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
     </row>
     <row r="13" ht="13.5" customHeight="1">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
     </row>
     <row r="14" ht="13.5" customHeight="1">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
     </row>
     <row r="15" ht="13.5" customHeight="1">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
-      <c r="N15" s="6"/>
-      <c r="O15" s="6"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
     </row>
     <row r="16" ht="13.5" customHeight="1">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
     </row>
     <row r="17" ht="13.5" customHeight="1">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="6"/>
-      <c r="O17" s="6"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
     </row>
     <row r="18" ht="13.5" customHeight="1">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="5"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
     </row>
     <row r="19" ht="13.5" customHeight="1">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
-      <c r="O19" s="6"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
     </row>
     <row r="20" ht="13.5" customHeight="1">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
-      <c r="O20" s="6"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
     </row>
     <row r="21" ht="13.5" customHeight="1">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="5"/>
-      <c r="O21" s="5"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
     </row>
     <row r="22" ht="13.5" customHeight="1">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="6"/>
-      <c r="M22" s="6"/>
-      <c r="N22" s="6"/>
-      <c r="O22" s="6"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7"/>
+      <c r="N22" s="7"/>
+      <c r="O22" s="7"/>
     </row>
     <row r="23" ht="13.5" customHeight="1">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
-      <c r="M23" s="6"/>
-      <c r="N23" s="6"/>
-      <c r="O23" s="6"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="7"/>
     </row>
     <row r="24" ht="13.5" customHeight="1">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
-      <c r="L24" s="6"/>
-      <c r="M24" s="6"/>
-      <c r="N24" s="6"/>
-      <c r="O24" s="6"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7"/>
     </row>
     <row r="25" ht="13.5" customHeight="1">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="6">
+      <c r="B25" s="7">
         <v>30.0</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25" s="7">
         <v>30.0</v>
       </c>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
-      <c r="L25" s="6"/>
-      <c r="M25" s="6"/>
-      <c r="N25" s="6"/>
-      <c r="O25" s="6"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="7"/>
+      <c r="O25" s="7"/>
     </row>
     <row r="26" ht="13.5" customHeight="1">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="6"/>
-      <c r="L26" s="6"/>
-      <c r="M26" s="6"/>
-      <c r="N26" s="6"/>
-      <c r="O26" s="6"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="7"/>
     </row>
     <row r="27" ht="13.5" customHeight="1">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B27" s="3"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
-      <c r="J27" s="5"/>
-      <c r="K27" s="5"/>
-      <c r="L27" s="5"/>
-      <c r="M27" s="5"/>
-      <c r="N27" s="5"/>
-      <c r="O27" s="5"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="6"/>
+      <c r="M27" s="6"/>
+      <c r="N27" s="6"/>
+      <c r="O27" s="6"/>
     </row>
     <row r="28" ht="13.5" customHeight="1">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6"/>
-      <c r="K28" s="6"/>
-      <c r="L28" s="6"/>
-      <c r="M28" s="6"/>
-      <c r="N28" s="6"/>
-      <c r="O28" s="6"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="7"/>
+      <c r="O28" s="7"/>
     </row>
     <row r="29" ht="13.5" customHeight="1">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="6"/>
-      <c r="K29" s="6"/>
-      <c r="L29" s="6"/>
-      <c r="M29" s="6"/>
-      <c r="N29" s="6"/>
-      <c r="O29" s="6"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="7"/>
+      <c r="N29" s="7"/>
+      <c r="O29" s="7"/>
     </row>
     <row r="30" ht="13.5" customHeight="1">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
-      <c r="J30" s="6"/>
-      <c r="K30" s="6"/>
-      <c r="L30" s="6"/>
-      <c r="M30" s="6"/>
-      <c r="N30" s="6"/>
-      <c r="O30" s="6"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
+      <c r="L30" s="7"/>
+      <c r="M30" s="7"/>
+      <c r="N30" s="7"/>
+      <c r="O30" s="7"/>
     </row>
     <row r="31" ht="13.5" customHeight="1">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="6"/>
-      <c r="K31" s="6"/>
-      <c r="L31" s="6"/>
-      <c r="M31" s="6"/>
-      <c r="N31" s="6"/>
-      <c r="O31" s="6"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="7"/>
+      <c r="L31" s="7"/>
+      <c r="M31" s="7"/>
+      <c r="N31" s="7"/>
+      <c r="O31" s="7"/>
     </row>
     <row r="32" ht="13.5" customHeight="1">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B32" s="3"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
-      <c r="I32" s="5"/>
-      <c r="J32" s="5"/>
-      <c r="K32" s="5"/>
-      <c r="L32" s="5"/>
-      <c r="M32" s="5"/>
-      <c r="N32" s="5"/>
-      <c r="O32" s="5"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="6"/>
+      <c r="M32" s="6"/>
+      <c r="N32" s="6"/>
+      <c r="O32" s="6"/>
     </row>
     <row r="33" ht="13.5" customHeight="1">
-      <c r="A33" s="6" t="s">
+      <c r="A33" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="C33" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="6"/>
-      <c r="J33" s="6"/>
-      <c r="K33" s="6"/>
-      <c r="L33" s="6"/>
-      <c r="M33" s="6"/>
-      <c r="N33" s="6"/>
-      <c r="O33" s="6"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="7"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="7"/>
     </row>
     <row r="34" ht="13.5" customHeight="1">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C34" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
-      <c r="J34" s="6"/>
-      <c r="K34" s="6"/>
-      <c r="L34" s="6"/>
-      <c r="M34" s="6"/>
-      <c r="N34" s="6"/>
-      <c r="O34" s="6"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
+      <c r="L34" s="7"/>
+      <c r="M34" s="7"/>
+      <c r="N34" s="7"/>
+      <c r="O34" s="7"/>
     </row>
     <row r="35" ht="13.5" customHeight="1">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B35" s="3"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="5"/>
-      <c r="I35" s="5"/>
-      <c r="J35" s="5"/>
-      <c r="K35" s="5"/>
-      <c r="L35" s="5"/>
-      <c r="M35" s="5"/>
-      <c r="N35" s="5"/>
-      <c r="O35" s="5"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
+      <c r="K35" s="6"/>
+      <c r="L35" s="6"/>
+      <c r="M35" s="6"/>
+      <c r="N35" s="6"/>
+      <c r="O35" s="6"/>
     </row>
     <row r="36" ht="13.5" customHeight="1">
-      <c r="A36" s="6" t="s">
+      <c r="A36" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
-      <c r="I36" s="6"/>
-      <c r="J36" s="6"/>
-      <c r="K36" s="6"/>
-      <c r="L36" s="6"/>
-      <c r="M36" s="6"/>
-      <c r="N36" s="6"/>
-      <c r="O36" s="6"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="7"/>
+      <c r="K36" s="7"/>
+      <c r="L36" s="7"/>
+      <c r="M36" s="7"/>
+      <c r="N36" s="7"/>
+      <c r="O36" s="7"/>
     </row>
     <row r="37" ht="13.5" customHeight="1">
-      <c r="A37" s="6" t="s">
+      <c r="A37" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="6"/>
-      <c r="J37" s="6"/>
-      <c r="K37" s="6"/>
-      <c r="L37" s="6"/>
-      <c r="M37" s="6"/>
-      <c r="N37" s="6"/>
-      <c r="O37" s="6"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
+      <c r="I37" s="7"/>
+      <c r="J37" s="7"/>
+      <c r="K37" s="7"/>
+      <c r="L37" s="7"/>
+      <c r="M37" s="7"/>
+      <c r="N37" s="7"/>
+      <c r="O37" s="7"/>
     </row>
     <row r="38" ht="13.5" customHeight="1">
-      <c r="A38" s="6" t="s">
+      <c r="A38" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="6"/>
-      <c r="H38" s="6"/>
-      <c r="I38" s="6"/>
-      <c r="J38" s="6"/>
-      <c r="K38" s="6"/>
-      <c r="L38" s="6"/>
-      <c r="M38" s="6"/>
-      <c r="N38" s="6"/>
-      <c r="O38" s="6"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="7"/>
+      <c r="K38" s="7"/>
+      <c r="L38" s="7"/>
+      <c r="M38" s="7"/>
+      <c r="N38" s="7"/>
+      <c r="O38" s="7"/>
     </row>
     <row r="39" ht="13.5" customHeight="1">
-      <c r="A39" s="6" t="s">
+      <c r="A39" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6"/>
-      <c r="I39" s="6"/>
-      <c r="J39" s="6"/>
-      <c r="K39" s="6"/>
-      <c r="L39" s="6"/>
-      <c r="M39" s="6"/>
-      <c r="N39" s="6"/>
-      <c r="O39" s="6"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
+      <c r="I39" s="7"/>
+      <c r="J39" s="7"/>
+      <c r="K39" s="7"/>
+      <c r="L39" s="7"/>
+      <c r="M39" s="7"/>
+      <c r="N39" s="7"/>
+      <c r="O39" s="7"/>
     </row>
     <row r="40" ht="13.5" customHeight="1">
-      <c r="A40" s="6" t="s">
+      <c r="A40" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="B40" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
-      <c r="G40" s="6"/>
-      <c r="H40" s="6"/>
-      <c r="I40" s="6"/>
-      <c r="J40" s="6"/>
-      <c r="K40" s="6"/>
-      <c r="L40" s="6"/>
-      <c r="M40" s="6"/>
-      <c r="N40" s="6"/>
-      <c r="O40" s="6"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
+      <c r="J40" s="7"/>
+      <c r="K40" s="7"/>
+      <c r="L40" s="7"/>
+      <c r="M40" s="7"/>
+      <c r="N40" s="7"/>
+      <c r="O40" s="7"/>
     </row>
     <row r="41" ht="13.5" customHeight="1">
-      <c r="A41" s="6" t="s">
+      <c r="A41" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B41" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="6"/>
-      <c r="H41" s="6"/>
-      <c r="I41" s="6"/>
-      <c r="J41" s="6"/>
-      <c r="K41" s="6"/>
-      <c r="L41" s="6"/>
-      <c r="M41" s="6"/>
-      <c r="N41" s="6"/>
-      <c r="O41" s="6"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="7"/>
+      <c r="J41" s="7"/>
+      <c r="K41" s="7"/>
+      <c r="L41" s="7"/>
+      <c r="M41" s="7"/>
+      <c r="N41" s="7"/>
+      <c r="O41" s="7"/>
     </row>
     <row r="42" ht="13.5" customHeight="1">
-      <c r="A42" s="2" t="s">
+      <c r="A42" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B42" s="3"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
-      <c r="G42" s="5"/>
-      <c r="H42" s="5"/>
-      <c r="I42" s="5"/>
-      <c r="J42" s="5"/>
-      <c r="K42" s="5"/>
-      <c r="L42" s="5"/>
-      <c r="M42" s="5"/>
-      <c r="N42" s="5"/>
-      <c r="O42" s="5"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="6"/>
+      <c r="I42" s="6"/>
+      <c r="J42" s="6"/>
+      <c r="K42" s="6"/>
+      <c r="L42" s="6"/>
+      <c r="M42" s="6"/>
+      <c r="N42" s="6"/>
+      <c r="O42" s="6"/>
     </row>
     <row r="43" ht="13.5" customHeight="1">
-      <c r="A43" s="6" t="s">
+      <c r="A43" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="B43" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C43" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="D43" s="6" t="s">
+      <c r="D43" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="E43" s="6" t="s">
+      <c r="E43" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="F43" s="6"/>
-      <c r="G43" s="6"/>
-      <c r="H43" s="6"/>
-      <c r="I43" s="6"/>
-      <c r="J43" s="6"/>
-      <c r="K43" s="6"/>
-      <c r="L43" s="6"/>
-      <c r="M43" s="6"/>
-      <c r="N43" s="6"/>
-      <c r="O43" s="6"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
+      <c r="I43" s="7"/>
+      <c r="J43" s="7"/>
+      <c r="K43" s="7"/>
+      <c r="L43" s="7"/>
+      <c r="M43" s="7"/>
+      <c r="N43" s="7"/>
+      <c r="O43" s="7"/>
     </row>
     <row r="44" ht="13.5" customHeight="1">
-      <c r="A44" s="6" t="s">
+      <c r="A44" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="B44" s="6" t="s">
+      <c r="B44" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="C44" s="6" t="s">
+      <c r="C44" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D44" s="6" t="s">
+      <c r="D44" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="E44" s="6" t="s">
+      <c r="E44" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="F44" s="6"/>
-      <c r="G44" s="6"/>
-      <c r="H44" s="6"/>
-      <c r="I44" s="6"/>
-      <c r="J44" s="6"/>
-      <c r="K44" s="6"/>
-      <c r="L44" s="6"/>
-      <c r="M44" s="6"/>
-      <c r="N44" s="6"/>
-      <c r="O44" s="6"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7"/>
+      <c r="I44" s="7"/>
+      <c r="J44" s="7"/>
+      <c r="K44" s="7"/>
+      <c r="L44" s="7"/>
+      <c r="M44" s="7"/>
+      <c r="N44" s="7"/>
+      <c r="O44" s="7"/>
     </row>
     <row r="45" ht="13.5" customHeight="1">
-      <c r="A45" s="2" t="s">
+      <c r="A45" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B45" s="3"/>
-      <c r="C45" s="4"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="5"/>
-      <c r="F45" s="5"/>
-      <c r="G45" s="5"/>
-      <c r="H45" s="5"/>
-      <c r="I45" s="5"/>
-      <c r="J45" s="5"/>
-      <c r="K45" s="5"/>
-      <c r="L45" s="5"/>
-      <c r="M45" s="5"/>
-      <c r="N45" s="5"/>
-      <c r="O45" s="5"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="6"/>
+      <c r="I45" s="6"/>
+      <c r="J45" s="6"/>
+      <c r="K45" s="6"/>
+      <c r="L45" s="6"/>
+      <c r="M45" s="6"/>
+      <c r="N45" s="6"/>
+      <c r="O45" s="6"/>
     </row>
     <row r="46" ht="13.5" customHeight="1">
-      <c r="A46" s="6" t="s">
+      <c r="A46" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="B46" s="6" t="s">
+      <c r="B46" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="6"/>
-      <c r="G46" s="6"/>
-      <c r="H46" s="6"/>
-      <c r="I46" s="6"/>
-      <c r="J46" s="6"/>
-      <c r="K46" s="6"/>
-      <c r="L46" s="6"/>
-      <c r="M46" s="6"/>
-      <c r="N46" s="6"/>
-      <c r="O46" s="6"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="7"/>
+      <c r="H46" s="7"/>
+      <c r="I46" s="7"/>
+      <c r="J46" s="7"/>
+      <c r="K46" s="7"/>
+      <c r="L46" s="7"/>
+      <c r="M46" s="7"/>
+      <c r="N46" s="7"/>
+      <c r="O46" s="7"/>
     </row>
     <row r="47" ht="13.5" customHeight="1">
-      <c r="A47" s="6" t="s">
+      <c r="A47" s="7" t="s">
         <v>95</v>
       </c>
       <c r="B47" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="6"/>
-      <c r="F47" s="6"/>
-      <c r="G47" s="6"/>
-      <c r="H47" s="6"/>
-      <c r="I47" s="6"/>
-      <c r="J47" s="6"/>
-      <c r="K47" s="6"/>
-      <c r="L47" s="6"/>
-      <c r="M47" s="6"/>
-      <c r="N47" s="6"/>
-      <c r="O47" s="6"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="7"/>
+      <c r="I47" s="7"/>
+      <c r="J47" s="7"/>
+      <c r="K47" s="7"/>
+      <c r="L47" s="7"/>
+      <c r="M47" s="7"/>
+      <c r="N47" s="7"/>
+      <c r="O47" s="7"/>
     </row>
     <row r="48" ht="13.5" customHeight="1">
       <c r="A48" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="B48" s="3"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="5"/>
-      <c r="F48" s="5"/>
-      <c r="G48" s="5"/>
-      <c r="H48" s="5"/>
-      <c r="I48" s="5"/>
-      <c r="J48" s="5"/>
-      <c r="K48" s="5"/>
-      <c r="L48" s="5"/>
-      <c r="M48" s="5"/>
-      <c r="N48" s="5"/>
-      <c r="O48" s="5"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="6"/>
+      <c r="I48" s="6"/>
+      <c r="J48" s="6"/>
+      <c r="K48" s="6"/>
+      <c r="L48" s="6"/>
+      <c r="M48" s="6"/>
+      <c r="N48" s="6"/>
+      <c r="O48" s="6"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="10" t="s">
@@ -1563,20 +1599,20 @@
       <c r="A54" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="B54" s="3"/>
-      <c r="C54" s="4"/>
-      <c r="D54" s="5"/>
-      <c r="E54" s="5"/>
-      <c r="F54" s="5"/>
-      <c r="G54" s="5"/>
-      <c r="H54" s="5"/>
-      <c r="I54" s="5"/>
-      <c r="J54" s="5"/>
-      <c r="K54" s="5"/>
-      <c r="L54" s="5"/>
-      <c r="M54" s="5"/>
-      <c r="N54" s="5"/>
-      <c r="O54" s="5"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
+      <c r="H54" s="6"/>
+      <c r="I54" s="6"/>
+      <c r="J54" s="6"/>
+      <c r="K54" s="6"/>
+      <c r="L54" s="6"/>
+      <c r="M54" s="6"/>
+      <c r="N54" s="6"/>
+      <c r="O54" s="6"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
       <c r="A55" s="10" t="s">
@@ -1610,12 +1646,54 @@
         <v>115</v>
       </c>
     </row>
-    <row r="59" ht="15.75" customHeight="1"/>
-    <row r="60" ht="15.75" customHeight="1"/>
-    <row r="61" ht="15.75" customHeight="1"/>
-    <row r="62" ht="15.75" customHeight="1"/>
-    <row r="63" ht="15.75" customHeight="1"/>
-    <row r="64" ht="15.75" customHeight="1"/>
+    <row r="59" ht="15.75" customHeight="1">
+      <c r="A59" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="60" ht="15.75" customHeight="1">
+      <c r="A60" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="61" ht="15.75" customHeight="1">
+      <c r="A61" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="B61" s="11" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="62" ht="15.75" customHeight="1">
+      <c r="A62" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="B62" s="11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="63" ht="15.75" customHeight="1">
+      <c r="A63" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B63" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="64" ht="15.75" customHeight="1">
+      <c r="A64" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
     <row r="65" ht="15.75" customHeight="1"/>
     <row r="66" ht="15.75" customHeight="1"/>
     <row r="67" ht="15.75" customHeight="1"/>
@@ -2593,79 +2671,79 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
     </row>
     <row r="2">
-      <c r="A2" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
     </row>
     <row r="3">
-      <c r="A3" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
     </row>
     <row r="4">
-      <c r="A4" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
     </row>
     <row r="5">
-      <c r="A5" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
+      <c r="A5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Added new test cases ScheduleDashboardTest.java Added new functions AllContent_Dahboard.java Updated functions name Updated TestData file
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/sendDashboard/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/sendDashboard/TestData.xlsx
@@ -12,59 +12,59 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="147">
   <si>
     <t>Supported Browser Types</t>
   </si>
   <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Data1</t>
+  </si>
+  <si>
+    <t>Data2</t>
+  </si>
+  <si>
+    <t>Data3</t>
+  </si>
+  <si>
+    <t>Data4</t>
+  </si>
+  <si>
+    <t>URLs</t>
+  </si>
+  <si>
     <t>MozillaFirefox</t>
   </si>
   <si>
-    <t>Variable</t>
+    <t>URL_login_login</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>URL_content_allContent</t>
+  </si>
+  <si>
+    <t>all-content/0</t>
+  </si>
+  <si>
+    <t>URL_security_groups</t>
+  </si>
+  <si>
+    <t>security/groups</t>
   </si>
   <si>
     <t>GoogleChrome</t>
   </si>
   <si>
-    <t>Data1</t>
-  </si>
-  <si>
     <t>MicrosoftInternetExplorer</t>
   </si>
   <si>
-    <t>Data2</t>
-  </si>
-  <si>
-    <t>Data3</t>
-  </si>
-  <si>
-    <t>Data4</t>
-  </si>
-  <si>
     <t>MicrosoftEdge</t>
   </si>
   <si>
-    <t>URLs</t>
-  </si>
-  <si>
-    <t>URL_login_login</t>
-  </si>
-  <si>
-    <t>login</t>
-  </si>
-  <si>
-    <t>URL_content_allContent</t>
-  </si>
-  <si>
-    <t>all-content/0</t>
-  </si>
-  <si>
-    <t>URL_security_groups</t>
-  </si>
-  <si>
-    <t>security/groups</t>
-  </si>
-  <si>
     <t>URL_security_users</t>
   </si>
   <si>
@@ -435,6 +435,24 @@
   </si>
   <si>
     <t>JobNameSaveChanges</t>
+  </si>
+  <si>
+    <t>ArabicSubject</t>
+  </si>
+  <si>
+    <t>أحمد</t>
+  </si>
+  <si>
+    <t>SpecialCharactersSubject</t>
+  </si>
+  <si>
+    <t>@Automation_1$#</t>
+  </si>
+  <si>
+    <t>LongBody</t>
+  </si>
+  <si>
+    <t>Hello this is created as an automation testing for long body name to be successfully accepted by Incorta system Hello this is created as an automation testing for long subject name to be successfully accepted by Incorta system</t>
   </si>
 </sst>
 </file>
@@ -513,7 +531,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -545,6 +563,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -581,19 +602,19 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -608,7 +629,7 @@
     </row>
     <row r="2" ht="13.5" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="5"/>
@@ -627,10 +648,10 @@
     </row>
     <row r="3" ht="13.5" customHeight="1">
       <c r="A3" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
@@ -648,10 +669,10 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
@@ -669,10 +690,10 @@
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="A5" s="7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
@@ -1793,10 +1814,29 @@
       </c>
     </row>
     <row r="72" ht="15.75" customHeight="1">
-      <c r="B72" s="10"/>
-    </row>
-    <row r="73" ht="15.75" customHeight="1"/>
-    <row r="74" ht="15.75" customHeight="1"/>
+      <c r="A72" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="B72" s="12" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="73" ht="15.75" customHeight="1">
+      <c r="A73" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="B73" s="10" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="74" ht="15.75" customHeight="1">
+      <c r="A74" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="B74" s="10" t="s">
+        <v>146</v>
+      </c>
+    </row>
     <row r="75" ht="15.75" customHeight="1"/>
     <row r="76" ht="15.75" customHeight="1"/>
     <row r="77" ht="15.75" customHeight="1"/>
@@ -2780,7 +2820,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2795,7 +2835,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -2810,7 +2850,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -2825,7 +2865,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>

</xml_diff>

<commit_message>
Updating scripts and updating testdata file
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/sendDashboard/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/sendDashboard/TestData.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="149">
   <si>
     <t>Supported Browser Types</t>
   </si>
@@ -20,6 +20,9 @@
     <t>Variable</t>
   </si>
   <si>
+    <t>MozillaFirefox</t>
+  </si>
+  <si>
     <t>Data1</t>
   </si>
   <si>
@@ -32,10 +35,16 @@
     <t>Data4</t>
   </si>
   <si>
+    <t>GoogleChrome</t>
+  </si>
+  <si>
+    <t>MicrosoftInternetExplorer</t>
+  </si>
+  <si>
     <t>URLs</t>
   </si>
   <si>
-    <t>MozillaFirefox</t>
+    <t>MicrosoftEdge</t>
   </si>
   <si>
     <t>URL_login_login</t>
@@ -56,15 +65,6 @@
     <t>security/groups</t>
   </si>
   <si>
-    <t>GoogleChrome</t>
-  </si>
-  <si>
-    <t>MicrosoftInternetExplorer</t>
-  </si>
-  <si>
-    <t>MicrosoftEdge</t>
-  </si>
-  <si>
     <t>URL_security_users</t>
   </si>
   <si>
@@ -453,6 +453,13 @@
   </si>
   <si>
     <t>Hello this is created as an automation testing for long body name to be successfully accepted by Incorta system Hello this is created as an automation testing for long subject name to be successfully accepted by Incorta system</t>
+  </si>
+  <si>
+    <t>BodyWithSpacesAndEnter</t>
+  </si>
+  <si>
+    <t>Automation
+New Automation</t>
   </si>
 </sst>
 </file>
@@ -605,16 +612,16 @@
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -629,7 +636,7 @@
     </row>
     <row r="2" ht="13.5" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="5"/>
@@ -648,10 +655,10 @@
     </row>
     <row r="3" ht="13.5" customHeight="1">
       <c r="A3" s="7" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
@@ -669,10 +676,10 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="7" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
@@ -690,10 +697,10 @@
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="A5" s="7" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
@@ -1837,7 +1844,14 @@
         <v>146</v>
       </c>
     </row>
-    <row r="75" ht="15.75" customHeight="1"/>
+    <row r="75" ht="15.75" customHeight="1">
+      <c r="A75" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="B75" s="10" t="s">
+        <v>148</v>
+      </c>
+    </row>
     <row r="76" ht="15.75" customHeight="1"/>
     <row r="77" ht="15.75" customHeight="1"/>
     <row r="78" ht="15.75" customHeight="1"/>
@@ -2820,7 +2834,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2835,7 +2849,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -2850,7 +2864,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -2865,7 +2879,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>

</xml_diff>

<commit_message>
Adding two test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/sendDashboard/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/sendDashboard/TestData.xlsx
@@ -12,14 +12,26 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="137">
+  <si>
+    <t>Supported Browser Types</t>
+  </si>
+  <si>
+    <t>MozillaFirefox</t>
+  </si>
+  <si>
+    <t>GoogleChrome</t>
+  </si>
+  <si>
+    <t>MicrosoftInternetExplorer</t>
+  </si>
+  <si>
+    <t>MicrosoftEdge</t>
+  </si>
   <si>
     <t>Variable</t>
   </si>
   <si>
-    <t>Supported Browser Types</t>
-  </si>
-  <si>
     <t>Data1</t>
   </si>
   <si>
@@ -35,18 +47,6 @@
     <t>URLs</t>
   </si>
   <si>
-    <t>MozillaFirefox</t>
-  </si>
-  <si>
-    <t>GoogleChrome</t>
-  </si>
-  <si>
-    <t>MicrosoftInternetExplorer</t>
-  </si>
-  <si>
-    <t>MicrosoftEdge</t>
-  </si>
-  <si>
     <t>URL_login_login</t>
   </si>
   <si>
@@ -318,6 +318,15 @@
   </si>
   <si>
     <t>@#$^&amp;*</t>
+  </si>
+  <si>
+    <t>NonEnglish</t>
+  </si>
+  <si>
+    <t>測試</t>
+  </si>
+  <si>
+    <t>Numbers</t>
   </si>
   <si>
     <t>Schedule Dashboard via email</t>
@@ -536,14 +545,14 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="2" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
@@ -638,35 +647,35 @@
   </cols>
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
     </row>
     <row r="2" ht="13.5" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="6"/>
@@ -1908,30 +1917,32 @@
       <c r="O55" s="16"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="A56" s="4" t="s">
+      <c r="A56" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="B56" s="5"/>
-      <c r="C56" s="6"/>
-      <c r="D56" s="19"/>
-      <c r="E56" s="19"/>
-      <c r="F56" s="20"/>
-      <c r="G56" s="20"/>
-      <c r="H56" s="20"/>
-      <c r="I56" s="20"/>
-      <c r="J56" s="20"/>
-      <c r="K56" s="20"/>
-      <c r="L56" s="20"/>
-      <c r="M56" s="20"/>
-      <c r="N56" s="20"/>
-      <c r="O56" s="20"/>
+      <c r="B56" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="C56" s="15"/>
+      <c r="D56" s="15"/>
+      <c r="E56" s="15"/>
+      <c r="F56" s="16"/>
+      <c r="G56" s="16"/>
+      <c r="H56" s="16"/>
+      <c r="I56" s="16"/>
+      <c r="J56" s="16"/>
+      <c r="K56" s="16"/>
+      <c r="L56" s="16"/>
+      <c r="M56" s="16"/>
+      <c r="N56" s="16"/>
+      <c r="O56" s="16"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
       <c r="A57" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="B57" s="14" t="s">
         <v>104</v>
+      </c>
+      <c r="B57" s="14">
+        <v>123456.0</v>
       </c>
       <c r="C57" s="15"/>
       <c r="D57" s="15"/>
@@ -1948,32 +1959,30 @@
       <c r="O57" s="16"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="14" t="s">
+      <c r="A58" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="B58" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="C58" s="15"/>
-      <c r="D58" s="15"/>
-      <c r="E58" s="15"/>
-      <c r="F58" s="16"/>
-      <c r="G58" s="16"/>
-      <c r="H58" s="16"/>
-      <c r="I58" s="16"/>
-      <c r="J58" s="16"/>
-      <c r="K58" s="16"/>
-      <c r="L58" s="16"/>
-      <c r="M58" s="16"/>
-      <c r="N58" s="16"/>
-      <c r="O58" s="16"/>
+      <c r="B58" s="5"/>
+      <c r="C58" s="6"/>
+      <c r="D58" s="19"/>
+      <c r="E58" s="19"/>
+      <c r="F58" s="20"/>
+      <c r="G58" s="20"/>
+      <c r="H58" s="20"/>
+      <c r="I58" s="20"/>
+      <c r="J58" s="20"/>
+      <c r="K58" s="20"/>
+      <c r="L58" s="20"/>
+      <c r="M58" s="20"/>
+      <c r="N58" s="20"/>
+      <c r="O58" s="20"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="B59" s="14" t="s">
         <v>107</v>
-      </c>
-      <c r="B59" s="14" t="s">
-        <v>108</v>
       </c>
       <c r="C59" s="15"/>
       <c r="D59" s="15"/>
@@ -1991,10 +2000,10 @@
     </row>
     <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="B60" s="14" t="s">
         <v>109</v>
-      </c>
-      <c r="B60" s="14" t="s">
-        <v>110</v>
       </c>
       <c r="C60" s="15"/>
       <c r="D60" s="15"/>
@@ -2012,10 +2021,10 @@
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="A61" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="B61" s="14" t="s">
         <v>111</v>
-      </c>
-      <c r="B61" s="14" t="s">
-        <v>112</v>
       </c>
       <c r="C61" s="15"/>
       <c r="D61" s="15"/>
@@ -2033,10 +2042,10 @@
     </row>
     <row r="62" ht="15.75" customHeight="1">
       <c r="A62" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="B62" s="14" t="s">
         <v>113</v>
-      </c>
-      <c r="B62" s="14" t="s">
-        <v>114</v>
       </c>
       <c r="C62" s="15"/>
       <c r="D62" s="15"/>
@@ -2054,10 +2063,10 @@
     </row>
     <row r="63" ht="15.75" customHeight="1">
       <c r="A63" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="B63" s="14" t="s">
         <v>115</v>
-      </c>
-      <c r="B63" s="17">
-        <v>44500.0</v>
       </c>
       <c r="C63" s="15"/>
       <c r="D63" s="15"/>
@@ -2077,8 +2086,8 @@
       <c r="A64" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="B64" s="18">
-        <v>0.6458333333333334</v>
+      <c r="B64" s="14" t="s">
+        <v>117</v>
       </c>
       <c r="C64" s="15"/>
       <c r="D64" s="15"/>
@@ -2096,10 +2105,10 @@
     </row>
     <row r="65" ht="15.75" customHeight="1">
       <c r="A65" s="14" t="s">
-        <v>117</v>
-      </c>
-      <c r="B65" s="14" t="s">
         <v>118</v>
+      </c>
+      <c r="B65" s="17">
+        <v>44500.0</v>
       </c>
       <c r="C65" s="15"/>
       <c r="D65" s="15"/>
@@ -2119,8 +2128,8 @@
       <c r="A66" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="B66" s="14" t="s">
-        <v>79</v>
+      <c r="B66" s="18">
+        <v>0.6458333333333334</v>
       </c>
       <c r="C66" s="15"/>
       <c r="D66" s="15"/>
@@ -2162,7 +2171,7 @@
         <v>122</v>
       </c>
       <c r="B68" s="14" t="s">
-        <v>123</v>
+        <v>79</v>
       </c>
       <c r="C68" s="15"/>
       <c r="D68" s="15"/>
@@ -2180,10 +2189,10 @@
     </row>
     <row r="69" ht="15.75" customHeight="1">
       <c r="A69" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="B69" s="14" t="s">
         <v>124</v>
-      </c>
-      <c r="B69" s="14" t="s">
-        <v>125</v>
       </c>
       <c r="C69" s="15"/>
       <c r="D69" s="15"/>
@@ -2201,10 +2210,10 @@
     </row>
     <row r="70" ht="15.75" customHeight="1">
       <c r="A70" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="B70" s="14" t="s">
         <v>126</v>
-      </c>
-      <c r="B70" s="14" t="s">
-        <v>127</v>
       </c>
       <c r="C70" s="15"/>
       <c r="D70" s="15"/>
@@ -2222,10 +2231,10 @@
     </row>
     <row r="71" ht="15.75" customHeight="1">
       <c r="A71" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="B71" s="14" t="s">
         <v>128</v>
-      </c>
-      <c r="B71" s="14" t="s">
-        <v>129</v>
       </c>
       <c r="C71" s="15"/>
       <c r="D71" s="15"/>
@@ -2243,10 +2252,10 @@
     </row>
     <row r="72" ht="15.75" customHeight="1">
       <c r="A72" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="B72" s="14" t="s">
         <v>130</v>
-      </c>
-      <c r="B72" s="14" t="s">
-        <v>131</v>
       </c>
       <c r="C72" s="15"/>
       <c r="D72" s="15"/>
@@ -2264,10 +2273,10 @@
     </row>
     <row r="73" ht="15.75" customHeight="1">
       <c r="A73" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="B73" s="14" t="s">
         <v>132</v>
-      </c>
-      <c r="B73" s="14" t="s">
-        <v>133</v>
       </c>
       <c r="C73" s="15"/>
       <c r="D73" s="15"/>
@@ -2284,11 +2293,15 @@
       <c r="O73" s="16"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
-      <c r="A74" s="16"/>
-      <c r="B74" s="16"/>
-      <c r="C74" s="16"/>
-      <c r="D74" s="16"/>
-      <c r="E74" s="16"/>
+      <c r="A74" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="B74" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="C74" s="15"/>
+      <c r="D74" s="15"/>
+      <c r="E74" s="15"/>
       <c r="F74" s="16"/>
       <c r="G74" s="16"/>
       <c r="H74" s="16"/>
@@ -2300,8 +2313,44 @@
       <c r="N74" s="16"/>
       <c r="O74" s="16"/>
     </row>
-    <row r="75" ht="15.75" customHeight="1"/>
-    <row r="76" ht="15.75" customHeight="1"/>
+    <row r="75" ht="15.75" customHeight="1">
+      <c r="A75" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="B75" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="C75" s="15"/>
+      <c r="D75" s="15"/>
+      <c r="E75" s="15"/>
+      <c r="F75" s="16"/>
+      <c r="G75" s="16"/>
+      <c r="H75" s="16"/>
+      <c r="I75" s="16"/>
+      <c r="J75" s="16"/>
+      <c r="K75" s="16"/>
+      <c r="L75" s="16"/>
+      <c r="M75" s="16"/>
+      <c r="N75" s="16"/>
+      <c r="O75" s="16"/>
+    </row>
+    <row r="76" ht="15.75" customHeight="1">
+      <c r="A76" s="16"/>
+      <c r="B76" s="16"/>
+      <c r="C76" s="16"/>
+      <c r="D76" s="16"/>
+      <c r="E76" s="16"/>
+      <c r="F76" s="16"/>
+      <c r="G76" s="16"/>
+      <c r="H76" s="16"/>
+      <c r="I76" s="16"/>
+      <c r="J76" s="16"/>
+      <c r="K76" s="16"/>
+      <c r="L76" s="16"/>
+      <c r="M76" s="16"/>
+      <c r="N76" s="16"/>
+      <c r="O76" s="16"/>
+    </row>
     <row r="77" ht="15.75" customHeight="1"/>
     <row r="78" ht="15.75" customHeight="1"/>
     <row r="79" ht="15.75" customHeight="1"/>
@@ -3228,20 +3277,22 @@
     <row r="1000" ht="15.75" customHeight="1"/>
     <row r="1001" ht="15.75" customHeight="1"/>
     <row r="1002" ht="15.75" customHeight="1"/>
+    <row r="1003" ht="15.75" customHeight="1"/>
+    <row r="1004" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="12">
     <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="A58:C58"/>
     <mergeCell ref="A18:C18"/>
     <mergeCell ref="A21:C21"/>
     <mergeCell ref="A27:C27"/>
     <mergeCell ref="A35:C35"/>
     <mergeCell ref="A42:C42"/>
     <mergeCell ref="A45:C45"/>
-    <mergeCell ref="A48:C48"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A12:C12"/>
     <mergeCell ref="A32:C32"/>
-    <mergeCell ref="A56:C56"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="B47"/>
@@ -3268,79 +3319,79 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
push latest created TCs
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/sendDashboard/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/sendDashboard/TestData.xlsx
@@ -17,33 +17,33 @@
     <t>Supported Browser Types</t>
   </si>
   <si>
+    <t>Variable</t>
+  </si>
+  <si>
     <t>MozillaFirefox</t>
   </si>
   <si>
     <t>GoogleChrome</t>
   </si>
   <si>
+    <t>Data1</t>
+  </si>
+  <si>
+    <t>Data2</t>
+  </si>
+  <si>
+    <t>Data3</t>
+  </si>
+  <si>
+    <t>Data4</t>
+  </si>
+  <si>
     <t>MicrosoftInternetExplorer</t>
   </si>
   <si>
     <t>MicrosoftEdge</t>
   </si>
   <si>
-    <t>Variable</t>
-  </si>
-  <si>
-    <t>Data1</t>
-  </si>
-  <si>
-    <t>Data2</t>
-  </si>
-  <si>
-    <t>Data3</t>
-  </si>
-  <si>
-    <t>Data4</t>
-  </si>
-  <si>
     <t>URLs</t>
   </si>
   <si>
@@ -308,13 +308,13 @@
     <t>A CSV file will be sent only for the first table in this dashboard.</t>
   </si>
   <si>
-    <t>ArabicSubject</t>
+    <t>Arabic</t>
   </si>
   <si>
     <t>البريد الإلكتروني</t>
   </si>
   <si>
-    <t>SpecialCharactersSubject</t>
+    <t>SpecialCharacters</t>
   </si>
   <si>
     <t>@#$^&amp;*</t>
@@ -648,19 +648,19 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
@@ -3335,7 +3335,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -3350,7 +3350,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -3365,7 +3365,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -3380,7 +3380,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>

</xml_diff>

<commit_message>
Comments from Mohab is updated.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/sendDashboard/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/sendDashboard/TestData.xlsx
@@ -12,11 +12,26 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="174">
+  <si>
+    <t>Supported Browser Types</t>
+  </si>
   <si>
     <t>Variable</t>
   </si>
   <si>
+    <t>MozillaFirefox</t>
+  </si>
+  <si>
+    <t>GoogleChrome</t>
+  </si>
+  <si>
+    <t>MicrosoftInternetExplorer</t>
+  </si>
+  <si>
+    <t>MicrosoftEdge</t>
+  </si>
+  <si>
     <t>Data1</t>
   </si>
   <si>
@@ -32,9 +47,6 @@
     <t>URLs</t>
   </si>
   <si>
-    <t>Supported Browser Types</t>
-  </si>
-  <si>
     <t>URL_login_login</t>
   </si>
   <si>
@@ -314,10 +326,7 @@
     <t>Send Dashboard via email</t>
   </si>
   <si>
-    <t>DashboardName</t>
-  </si>
-  <si>
-    <t>Sending Dashboard</t>
+    <t>Automation_Scheduler_DashboardName</t>
   </si>
   <si>
     <t>HideNotificationToolTipText</t>
@@ -385,10 +394,7 @@
     <t>Schedule Dashboard via email</t>
   </si>
   <si>
-    <t>JobName</t>
-  </si>
-  <si>
-    <t>Duplicate Job Name</t>
+    <t>Automation_Scheduler_DuplicateJobName</t>
   </si>
   <si>
     <t>Email</t>
@@ -409,10 +415,7 @@
     <t>File names are appended with a timestamp when they are generated. Toggling this option off will remove the timestamp. If you are sending this to a shared folder, the file will be overwritten.</t>
   </si>
   <si>
-    <t>ScheduleJobName</t>
-  </si>
-  <si>
-    <t>UpdateJob</t>
+    <t>Automation_Scheduler_UpdateJobName</t>
   </si>
   <si>
     <t>ScheduleJobDescription</t>
@@ -424,9 +427,6 @@
     <t>ScheduleJobDate</t>
   </si>
   <si>
-    <t>MozillaFirefox</t>
-  </si>
-  <si>
     <t>10/31/2021</t>
   </si>
   <si>
@@ -451,9 +451,6 @@
     <t>Daily</t>
   </si>
   <si>
-    <t>GoogleChrome</t>
-  </si>
-  <si>
     <t>ScheduleJobWeeklyRecurrence</t>
   </si>
   <si>
@@ -466,34 +463,19 @@
     <t>Monthly</t>
   </si>
   <si>
-    <t>MicrosoftInternetExplorer</t>
-  </si>
-  <si>
     <t>LongSubjectName</t>
   </si>
   <si>
     <t>Hello this is created as an automation testing for long subject name to be successfully accepted by Incorta system</t>
   </si>
   <si>
-    <t>MicrosoftEdge</t>
-  </si>
-  <si>
-    <t>DeleteScheduleDashboard</t>
-  </si>
-  <si>
-    <t>DeleteJob</t>
-  </si>
-  <si>
-    <t>SuspendScheduleDashboard</t>
-  </si>
-  <si>
-    <t>SuspendJob</t>
-  </si>
-  <si>
-    <t>C77042JobName</t>
-  </si>
-  <si>
-    <t>JobNameSaveChanges</t>
+    <t>Automation_Schedule_DeleteJob</t>
+  </si>
+  <si>
+    <t>Automation_Schedule_SuspendJob</t>
+  </si>
+  <si>
+    <t>Automation_Scheduler_SaveChnages_JobName</t>
   </si>
   <si>
     <t>ArabicSubject</t>
@@ -657,6 +639,9 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -683,17 +668,14 @@
     <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -729,1441 +711,1441 @@
   </cols>
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
     </row>
     <row r="2" ht="13.5" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
+      <c r="A2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
     </row>
     <row r="3" ht="13.5" customHeight="1">
-      <c r="A3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
+      <c r="A3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
     </row>
     <row r="4" ht="13.5" customHeight="1">
-      <c r="A4" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
+      <c r="A4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
     </row>
     <row r="5" ht="13.5" customHeight="1">
-      <c r="A5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
+      <c r="A5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
     </row>
     <row r="6" ht="13.5" customHeight="1">
-      <c r="A6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
+      <c r="A6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
     </row>
     <row r="7" ht="13.5" customHeight="1">
-      <c r="A7" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
+      <c r="A7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
     </row>
     <row r="8" ht="13.5" customHeight="1">
-      <c r="A8" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
+      <c r="A8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
     </row>
     <row r="9" ht="13.5" customHeight="1">
-      <c r="A9" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
+      <c r="A9" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
     </row>
     <row r="10" ht="13.5" customHeight="1">
-      <c r="A10" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
+      <c r="A10" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
     </row>
     <row r="11" ht="13.5" customHeight="1">
-      <c r="A11" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
+      <c r="A11" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
     </row>
     <row r="12" ht="13.5" customHeight="1">
-      <c r="A12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
+      <c r="A12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
     </row>
     <row r="13" ht="13.5" customHeight="1">
-      <c r="A13" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
+      <c r="A13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
     </row>
     <row r="14" ht="13.5" customHeight="1">
-      <c r="A14" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
+      <c r="A14" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
     </row>
     <row r="15" ht="13.5" customHeight="1">
-      <c r="A15" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
-      <c r="N15" s="6"/>
-      <c r="O15" s="6"/>
+      <c r="A15" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
     </row>
     <row r="16" ht="13.5" customHeight="1">
-      <c r="A16" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
-      <c r="N16" s="6"/>
-      <c r="O16" s="6"/>
+      <c r="A16" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
     </row>
     <row r="17" ht="13.5" customHeight="1">
-      <c r="A17" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="6"/>
-      <c r="O17" s="6"/>
+      <c r="A17" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
     </row>
     <row r="18" ht="13.5" customHeight="1">
-      <c r="A18" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
-      <c r="N18" s="6"/>
-      <c r="O18" s="6"/>
+      <c r="A18" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
     </row>
     <row r="19" ht="13.5" customHeight="1">
-      <c r="A19" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
-      <c r="O19" s="6"/>
+      <c r="A19" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
     </row>
     <row r="20" ht="13.5" customHeight="1">
-      <c r="A20" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="5"/>
-      <c r="O20" s="5"/>
+      <c r="A20" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
     </row>
     <row r="21" ht="13.5" customHeight="1">
-      <c r="A21" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
-      <c r="N21" s="6"/>
-      <c r="O21" s="6"/>
+      <c r="A21" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="7"/>
     </row>
     <row r="22" ht="13.5" customHeight="1">
-      <c r="A22" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="5"/>
-      <c r="O22" s="5"/>
+      <c r="A22" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="6"/>
     </row>
     <row r="23" ht="13.5" customHeight="1">
-      <c r="A23" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
-      <c r="M23" s="6"/>
-      <c r="N23" s="6"/>
-      <c r="O23" s="6"/>
+      <c r="A23" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="7"/>
     </row>
     <row r="24" ht="13.5" customHeight="1">
-      <c r="A24" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
-      <c r="L24" s="6"/>
-      <c r="M24" s="6"/>
-      <c r="N24" s="6"/>
-      <c r="O24" s="6"/>
+      <c r="A24" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7"/>
     </row>
     <row r="25" ht="13.5" customHeight="1">
-      <c r="A25" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B25" s="3"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
-      <c r="L25" s="5"/>
-      <c r="M25" s="5"/>
-      <c r="N25" s="5"/>
-      <c r="O25" s="5"/>
+      <c r="A25" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="4"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="6"/>
+      <c r="O25" s="6"/>
     </row>
     <row r="26" ht="13.5" customHeight="1">
-      <c r="A26" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="6"/>
-      <c r="L26" s="6"/>
-      <c r="M26" s="6"/>
-      <c r="N26" s="6"/>
-      <c r="O26" s="6"/>
+      <c r="A26" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="7"/>
     </row>
     <row r="27" ht="13.5" customHeight="1">
-      <c r="A27" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="6"/>
-      <c r="K27" s="6"/>
-      <c r="L27" s="6"/>
-      <c r="M27" s="6"/>
-      <c r="N27" s="6"/>
-      <c r="O27" s="6"/>
+      <c r="A27" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="7"/>
+      <c r="N27" s="7"/>
+      <c r="O27" s="7"/>
     </row>
     <row r="28" ht="13.5" customHeight="1">
-      <c r="A28" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6"/>
-      <c r="K28" s="6"/>
-      <c r="L28" s="6"/>
-      <c r="M28" s="6"/>
-      <c r="N28" s="6"/>
-      <c r="O28" s="6"/>
+      <c r="A28" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="7"/>
+      <c r="O28" s="7"/>
     </row>
     <row r="29" ht="13.5" customHeight="1">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29" s="7">
+        <v>30.0</v>
+      </c>
+      <c r="C29" s="7">
+        <v>30.0</v>
+      </c>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="7"/>
+      <c r="N29" s="7"/>
+      <c r="O29" s="7"/>
+    </row>
+    <row r="30" ht="13.5" customHeight="1">
+      <c r="A30" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
+      <c r="L30" s="7"/>
+      <c r="M30" s="7"/>
+      <c r="N30" s="7"/>
+      <c r="O30" s="7"/>
+    </row>
+    <row r="31" ht="13.5" customHeight="1">
+      <c r="A31" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B31" s="4"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="6"/>
+      <c r="M31" s="6"/>
+      <c r="N31" s="6"/>
+      <c r="O31" s="6"/>
+    </row>
+    <row r="32" ht="13.5" customHeight="1">
+      <c r="A32" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="7"/>
+      <c r="K32" s="7"/>
+      <c r="L32" s="7"/>
+      <c r="M32" s="7"/>
+      <c r="N32" s="7"/>
+      <c r="O32" s="7"/>
+    </row>
+    <row r="33" ht="13.5" customHeight="1">
+      <c r="A33" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="7"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="7"/>
+    </row>
+    <row r="34" ht="13.5" customHeight="1">
+      <c r="A34" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
+      <c r="L34" s="7"/>
+      <c r="M34" s="7"/>
+      <c r="N34" s="7"/>
+      <c r="O34" s="7"/>
+    </row>
+    <row r="35" ht="13.5" customHeight="1">
+      <c r="A35" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
+      <c r="L35" s="7"/>
+      <c r="M35" s="7"/>
+      <c r="N35" s="7"/>
+      <c r="O35" s="7"/>
+    </row>
+    <row r="36" ht="13.5" customHeight="1">
+      <c r="A36" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B36" s="4"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="6"/>
+      <c r="K36" s="6"/>
+      <c r="L36" s="6"/>
+      <c r="M36" s="6"/>
+      <c r="N36" s="6"/>
+      <c r="O36" s="6"/>
+    </row>
+    <row r="37" ht="13.5" customHeight="1">
+      <c r="A37" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B37" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B29" s="6">
-        <v>30.0</v>
-      </c>
-      <c r="C29" s="6">
-        <v>30.0</v>
-      </c>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="6"/>
-      <c r="K29" s="6"/>
-      <c r="L29" s="6"/>
-      <c r="M29" s="6"/>
-      <c r="N29" s="6"/>
-      <c r="O29" s="6"/>
-    </row>
-    <row r="30" ht="13.5" customHeight="1">
-      <c r="A30" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
-      <c r="J30" s="6"/>
-      <c r="K30" s="6"/>
-      <c r="L30" s="6"/>
-      <c r="M30" s="6"/>
-      <c r="N30" s="6"/>
-      <c r="O30" s="6"/>
-    </row>
-    <row r="31" ht="13.5" customHeight="1">
-      <c r="A31" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B31" s="3"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="5"/>
-      <c r="L31" s="5"/>
-      <c r="M31" s="5"/>
-      <c r="N31" s="5"/>
-      <c r="O31" s="5"/>
-    </row>
-    <row r="32" ht="13.5" customHeight="1">
-      <c r="A32" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="6"/>
-      <c r="J32" s="6"/>
-      <c r="K32" s="6"/>
-      <c r="L32" s="6"/>
-      <c r="M32" s="6"/>
-      <c r="N32" s="6"/>
-      <c r="O32" s="6"/>
-    </row>
-    <row r="33" ht="13.5" customHeight="1">
-      <c r="A33" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="6"/>
-      <c r="J33" s="6"/>
-      <c r="K33" s="6"/>
-      <c r="L33" s="6"/>
-      <c r="M33" s="6"/>
-      <c r="N33" s="6"/>
-      <c r="O33" s="6"/>
-    </row>
-    <row r="34" ht="13.5" customHeight="1">
-      <c r="A34" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
-      <c r="J34" s="6"/>
-      <c r="K34" s="6"/>
-      <c r="L34" s="6"/>
-      <c r="M34" s="6"/>
-      <c r="N34" s="6"/>
-      <c r="O34" s="6"/>
-    </row>
-    <row r="35" ht="13.5" customHeight="1">
-      <c r="A35" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="B35" s="6" t="s">
+      <c r="C37" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
+      <c r="I37" s="7"/>
+      <c r="J37" s="7"/>
+      <c r="K37" s="7"/>
+      <c r="L37" s="7"/>
+      <c r="M37" s="7"/>
+      <c r="N37" s="7"/>
+      <c r="O37" s="7"/>
+    </row>
+    <row r="38" ht="13.5" customHeight="1">
+      <c r="A38" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="7"/>
+      <c r="K38" s="7"/>
+      <c r="L38" s="7"/>
+      <c r="M38" s="7"/>
+      <c r="N38" s="7"/>
+      <c r="O38" s="7"/>
+    </row>
+    <row r="39" ht="13.5" customHeight="1">
+      <c r="A39" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" s="4"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="6"/>
+      <c r="J39" s="6"/>
+      <c r="K39" s="6"/>
+      <c r="L39" s="6"/>
+      <c r="M39" s="6"/>
+      <c r="N39" s="6"/>
+      <c r="O39" s="6"/>
+    </row>
+    <row r="40" ht="13.5" customHeight="1">
+      <c r="A40" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
+      <c r="J40" s="7"/>
+      <c r="K40" s="7"/>
+      <c r="L40" s="7"/>
+      <c r="M40" s="7"/>
+      <c r="N40" s="7"/>
+      <c r="O40" s="7"/>
+    </row>
+    <row r="41" ht="13.5" customHeight="1">
+      <c r="A41" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="7"/>
+      <c r="J41" s="7"/>
+      <c r="K41" s="7"/>
+      <c r="L41" s="7"/>
+      <c r="M41" s="7"/>
+      <c r="N41" s="7"/>
+      <c r="O41" s="7"/>
+    </row>
+    <row r="42" ht="13.5" customHeight="1">
+      <c r="A42" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="7"/>
+      <c r="I42" s="7"/>
+      <c r="J42" s="7"/>
+      <c r="K42" s="7"/>
+      <c r="L42" s="7"/>
+      <c r="M42" s="7"/>
+      <c r="N42" s="7"/>
+      <c r="O42" s="7"/>
+    </row>
+    <row r="43" ht="13.5" customHeight="1">
+      <c r="A43" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
+      <c r="I43" s="7"/>
+      <c r="J43" s="7"/>
+      <c r="K43" s="7"/>
+      <c r="L43" s="7"/>
+      <c r="M43" s="7"/>
+      <c r="N43" s="7"/>
+      <c r="O43" s="7"/>
+    </row>
+    <row r="44" ht="13.5" customHeight="1">
+      <c r="A44" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7"/>
+      <c r="I44" s="7"/>
+      <c r="J44" s="7"/>
+      <c r="K44" s="7"/>
+      <c r="L44" s="7"/>
+      <c r="M44" s="7"/>
+      <c r="N44" s="7"/>
+      <c r="O44" s="7"/>
+    </row>
+    <row r="45" ht="13.5" customHeight="1">
+      <c r="A45" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="7"/>
+      <c r="I45" s="7"/>
+      <c r="J45" s="7"/>
+      <c r="K45" s="7"/>
+      <c r="L45" s="7"/>
+      <c r="M45" s="7"/>
+      <c r="N45" s="7"/>
+      <c r="O45" s="7"/>
+    </row>
+    <row r="46" ht="13.5" customHeight="1">
+      <c r="A46" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B46" s="4"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="6"/>
+      <c r="I46" s="6"/>
+      <c r="J46" s="6"/>
+      <c r="K46" s="6"/>
+      <c r="L46" s="6"/>
+      <c r="M46" s="6"/>
+      <c r="N46" s="6"/>
+      <c r="O46" s="6"/>
+    </row>
+    <row r="47" ht="13.5" customHeight="1">
+      <c r="A47" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="7"/>
+      <c r="I47" s="7"/>
+      <c r="J47" s="7"/>
+      <c r="K47" s="7"/>
+      <c r="L47" s="7"/>
+      <c r="M47" s="7"/>
+      <c r="N47" s="7"/>
+      <c r="O47" s="7"/>
+    </row>
+    <row r="48" ht="13.5" customHeight="1">
+      <c r="A48" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="F48" s="7"/>
+      <c r="G48" s="7"/>
+      <c r="H48" s="7"/>
+      <c r="I48" s="7"/>
+      <c r="J48" s="7"/>
+      <c r="K48" s="7"/>
+      <c r="L48" s="7"/>
+      <c r="M48" s="7"/>
+      <c r="N48" s="7"/>
+      <c r="O48" s="7"/>
+    </row>
+    <row r="49" ht="13.5" customHeight="1">
+      <c r="A49" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B49" s="4"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6"/>
+      <c r="H49" s="6"/>
+      <c r="I49" s="6"/>
+      <c r="J49" s="6"/>
+      <c r="K49" s="6"/>
+      <c r="L49" s="6"/>
+      <c r="M49" s="6"/>
+      <c r="N49" s="6"/>
+      <c r="O49" s="6"/>
+    </row>
+    <row r="50" ht="13.5" customHeight="1">
+      <c r="A50" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C50" s="7"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="7"/>
+      <c r="H50" s="7"/>
+      <c r="I50" s="7"/>
+      <c r="J50" s="7"/>
+      <c r="K50" s="7"/>
+      <c r="L50" s="7"/>
+      <c r="M50" s="7"/>
+      <c r="N50" s="7"/>
+      <c r="O50" s="7"/>
+    </row>
+    <row r="51" ht="13.5" customHeight="1">
+      <c r="A51" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="C51" s="7"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7"/>
+      <c r="G51" s="7"/>
+      <c r="H51" s="7"/>
+      <c r="I51" s="7"/>
+      <c r="J51" s="7"/>
+      <c r="K51" s="7"/>
+      <c r="L51" s="7"/>
+      <c r="M51" s="7"/>
+      <c r="N51" s="7"/>
+      <c r="O51" s="7"/>
+    </row>
+    <row r="52" ht="13.5" customHeight="1">
+      <c r="A52" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="B52" s="4"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
+      <c r="H52" s="6"/>
+      <c r="I52" s="6"/>
+      <c r="J52" s="6"/>
+      <c r="K52" s="6"/>
+      <c r="L52" s="6"/>
+      <c r="M52" s="6"/>
+      <c r="N52" s="6"/>
+      <c r="O52" s="6"/>
+    </row>
+    <row r="53" ht="15.75" customHeight="1">
+      <c r="A53" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="54" ht="15.75" customHeight="1">
+      <c r="A54" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="55" ht="15.75" customHeight="1">
+      <c r="A55" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="56" ht="15.75" customHeight="1">
+      <c r="A56" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="57" ht="15.75" customHeight="1">
+      <c r="A57" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6"/>
-      <c r="I35" s="6"/>
-      <c r="J35" s="6"/>
-      <c r="K35" s="6"/>
-      <c r="L35" s="6"/>
-      <c r="M35" s="6"/>
-      <c r="N35" s="6"/>
-      <c r="O35" s="6"/>
-    </row>
-    <row r="36" ht="13.5" customHeight="1">
-      <c r="A36" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B36" s="3"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
-      <c r="I36" s="5"/>
-      <c r="J36" s="5"/>
-      <c r="K36" s="5"/>
-      <c r="L36" s="5"/>
-      <c r="M36" s="5"/>
-      <c r="N36" s="5"/>
-      <c r="O36" s="5"/>
-    </row>
-    <row r="37" ht="13.5" customHeight="1">
-      <c r="A37" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="6"/>
-      <c r="J37" s="6"/>
-      <c r="K37" s="6"/>
-      <c r="L37" s="6"/>
-      <c r="M37" s="6"/>
-      <c r="N37" s="6"/>
-      <c r="O37" s="6"/>
-    </row>
-    <row r="38" ht="13.5" customHeight="1">
-      <c r="A38" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="6"/>
-      <c r="H38" s="6"/>
-      <c r="I38" s="6"/>
-      <c r="J38" s="6"/>
-      <c r="K38" s="6"/>
-      <c r="L38" s="6"/>
-      <c r="M38" s="6"/>
-      <c r="N38" s="6"/>
-      <c r="O38" s="6"/>
-    </row>
-    <row r="39" ht="13.5" customHeight="1">
-      <c r="A39" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B39" s="3"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
-      <c r="H39" s="5"/>
-      <c r="I39" s="5"/>
-      <c r="J39" s="5"/>
-      <c r="K39" s="5"/>
-      <c r="L39" s="5"/>
-      <c r="M39" s="5"/>
-      <c r="N39" s="5"/>
-      <c r="O39" s="5"/>
-    </row>
-    <row r="40" ht="13.5" customHeight="1">
-      <c r="A40" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="B40" s="6"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
-      <c r="G40" s="6"/>
-      <c r="H40" s="6"/>
-      <c r="I40" s="6"/>
-      <c r="J40" s="6"/>
-      <c r="K40" s="6"/>
-      <c r="L40" s="6"/>
-      <c r="M40" s="6"/>
-      <c r="N40" s="6"/>
-      <c r="O40" s="6"/>
-    </row>
-    <row r="41" ht="13.5" customHeight="1">
-      <c r="A41" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B41" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="6"/>
-      <c r="H41" s="6"/>
-      <c r="I41" s="6"/>
-      <c r="J41" s="6"/>
-      <c r="K41" s="6"/>
-      <c r="L41" s="6"/>
-      <c r="M41" s="6"/>
-      <c r="N41" s="6"/>
-      <c r="O41" s="6"/>
-    </row>
-    <row r="42" ht="13.5" customHeight="1">
-      <c r="A42" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6"/>
-      <c r="H42" s="6"/>
-      <c r="I42" s="6"/>
-      <c r="J42" s="6"/>
-      <c r="K42" s="6"/>
-      <c r="L42" s="6"/>
-      <c r="M42" s="6"/>
-      <c r="N42" s="6"/>
-      <c r="O42" s="6"/>
-    </row>
-    <row r="43" ht="13.5" customHeight="1">
-      <c r="A43" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="C43" s="6"/>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
-      <c r="F43" s="6"/>
-      <c r="G43" s="6"/>
-      <c r="H43" s="6"/>
-      <c r="I43" s="6"/>
-      <c r="J43" s="6"/>
-      <c r="K43" s="6"/>
-      <c r="L43" s="6"/>
-      <c r="M43" s="6"/>
-      <c r="N43" s="6"/>
-      <c r="O43" s="6"/>
-    </row>
-    <row r="44" ht="13.5" customHeight="1">
-      <c r="A44" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C44" s="6"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="6"/>
-      <c r="G44" s="6"/>
-      <c r="H44" s="6"/>
-      <c r="I44" s="6"/>
-      <c r="J44" s="6"/>
-      <c r="K44" s="6"/>
-      <c r="L44" s="6"/>
-      <c r="M44" s="6"/>
-      <c r="N44" s="6"/>
-      <c r="O44" s="6"/>
-    </row>
-    <row r="45" ht="13.5" customHeight="1">
-      <c r="A45" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="6"/>
-      <c r="G45" s="6"/>
-      <c r="H45" s="6"/>
-      <c r="I45" s="6"/>
-      <c r="J45" s="6"/>
-      <c r="K45" s="6"/>
-      <c r="L45" s="6"/>
-      <c r="M45" s="6"/>
-      <c r="N45" s="6"/>
-      <c r="O45" s="6"/>
-    </row>
-    <row r="46" ht="13.5" customHeight="1">
-      <c r="A46" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B46" s="3"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5"/>
-      <c r="F46" s="5"/>
-      <c r="G46" s="5"/>
-      <c r="H46" s="5"/>
-      <c r="I46" s="5"/>
-      <c r="J46" s="5"/>
-      <c r="K46" s="5"/>
-      <c r="L46" s="5"/>
-      <c r="M46" s="5"/>
-      <c r="N46" s="5"/>
-      <c r="O46" s="5"/>
-    </row>
-    <row r="47" ht="13.5" customHeight="1">
-      <c r="A47" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="B47" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="C47" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="E47" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="F47" s="6"/>
-      <c r="G47" s="6"/>
-      <c r="H47" s="6"/>
-      <c r="I47" s="6"/>
-      <c r="J47" s="6"/>
-      <c r="K47" s="6"/>
-      <c r="L47" s="6"/>
-      <c r="M47" s="6"/>
-      <c r="N47" s="6"/>
-      <c r="O47" s="6"/>
-    </row>
-    <row r="48" ht="13.5" customHeight="1">
-      <c r="A48" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="C48" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="E48" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="F48" s="6"/>
-      <c r="G48" s="6"/>
-      <c r="H48" s="6"/>
-      <c r="I48" s="6"/>
-      <c r="J48" s="6"/>
-      <c r="K48" s="6"/>
-      <c r="L48" s="6"/>
-      <c r="M48" s="6"/>
-      <c r="N48" s="6"/>
-      <c r="O48" s="6"/>
-    </row>
-    <row r="49" ht="13.5" customHeight="1">
-      <c r="A49" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B49" s="3"/>
-      <c r="C49" s="4"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
-      <c r="G49" s="5"/>
-      <c r="H49" s="5"/>
-      <c r="I49" s="5"/>
-      <c r="J49" s="5"/>
-      <c r="K49" s="5"/>
-      <c r="L49" s="5"/>
-      <c r="M49" s="5"/>
-      <c r="N49" s="5"/>
-      <c r="O49" s="5"/>
-    </row>
-    <row r="50" ht="13.5" customHeight="1">
-      <c r="A50" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="B50" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="C50" s="6"/>
-      <c r="D50" s="6"/>
-      <c r="E50" s="6"/>
-      <c r="F50" s="6"/>
-      <c r="G50" s="6"/>
-      <c r="H50" s="6"/>
-      <c r="I50" s="6"/>
-      <c r="J50" s="6"/>
-      <c r="K50" s="6"/>
-      <c r="L50" s="6"/>
-      <c r="M50" s="6"/>
-      <c r="N50" s="6"/>
-      <c r="O50" s="6"/>
-    </row>
-    <row r="51" ht="13.5" customHeight="1">
-      <c r="A51" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="C51" s="6"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="6"/>
-      <c r="F51" s="6"/>
-      <c r="G51" s="6"/>
-      <c r="H51" s="6"/>
-      <c r="I51" s="6"/>
-      <c r="J51" s="6"/>
-      <c r="K51" s="6"/>
-      <c r="L51" s="6"/>
-      <c r="M51" s="6"/>
-      <c r="N51" s="6"/>
-      <c r="O51" s="6"/>
-    </row>
-    <row r="52" ht="13.5" customHeight="1">
-      <c r="A52" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="B52" s="3"/>
-      <c r="C52" s="4"/>
-      <c r="D52" s="5"/>
-      <c r="E52" s="5"/>
-      <c r="F52" s="5"/>
-      <c r="G52" s="5"/>
-      <c r="H52" s="5"/>
-      <c r="I52" s="5"/>
-      <c r="J52" s="5"/>
-      <c r="K52" s="5"/>
-      <c r="L52" s="5"/>
-      <c r="M52" s="5"/>
-      <c r="N52" s="5"/>
-      <c r="O52" s="5"/>
-    </row>
-    <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="B53" s="7" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="B54" s="7" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="55" ht="15.75" customHeight="1">
-      <c r="A55" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="B55" s="7" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="56" ht="15.75" customHeight="1">
-      <c r="A56" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="B56" s="7" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="B57" s="7" t="s">
-        <v>108</v>
+      <c r="B57" s="8" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="B58" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="C58" s="10"/>
-      <c r="D58" s="10"/>
-      <c r="E58" s="10"/>
-      <c r="F58" s="10"/>
-      <c r="G58" s="10"/>
-      <c r="H58" s="10"/>
-      <c r="I58" s="10"/>
-      <c r="J58" s="10"/>
-      <c r="K58" s="10"/>
-      <c r="L58" s="10"/>
-      <c r="M58" s="10"/>
-      <c r="N58" s="10"/>
-      <c r="O58" s="10"/>
-      <c r="P58" s="10"/>
-      <c r="Q58" s="10"/>
-      <c r="R58" s="10"/>
-      <c r="S58" s="10"/>
-      <c r="T58" s="10"/>
-      <c r="U58" s="10"/>
-      <c r="V58" s="10"/>
-      <c r="W58" s="10"/>
-      <c r="X58" s="10"/>
-      <c r="Y58" s="10"/>
-      <c r="Z58" s="10"/>
+      <c r="A58" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="C58" s="11"/>
+      <c r="D58" s="11"/>
+      <c r="E58" s="11"/>
+      <c r="F58" s="11"/>
+      <c r="G58" s="11"/>
+      <c r="H58" s="11"/>
+      <c r="I58" s="11"/>
+      <c r="J58" s="11"/>
+      <c r="K58" s="11"/>
+      <c r="L58" s="11"/>
+      <c r="M58" s="11"/>
+      <c r="N58" s="11"/>
+      <c r="O58" s="11"/>
+      <c r="P58" s="11"/>
+      <c r="Q58" s="11"/>
+      <c r="R58" s="11"/>
+      <c r="S58" s="11"/>
+      <c r="T58" s="11"/>
+      <c r="U58" s="11"/>
+      <c r="V58" s="11"/>
+      <c r="W58" s="11"/>
+      <c r="X58" s="11"/>
+      <c r="Y58" s="11"/>
+      <c r="Z58" s="11"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="B59" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="C59" s="10"/>
-      <c r="D59" s="10"/>
-      <c r="E59" s="10"/>
-      <c r="F59" s="10"/>
-      <c r="G59" s="10"/>
-      <c r="H59" s="10"/>
-      <c r="I59" s="10"/>
-      <c r="J59" s="10"/>
-      <c r="K59" s="10"/>
-      <c r="L59" s="10"/>
-      <c r="M59" s="10"/>
-      <c r="N59" s="10"/>
-      <c r="O59" s="10"/>
-      <c r="P59" s="10"/>
-      <c r="Q59" s="10"/>
-      <c r="R59" s="10"/>
-      <c r="S59" s="10"/>
-      <c r="T59" s="10"/>
-      <c r="U59" s="10"/>
-      <c r="V59" s="10"/>
-      <c r="W59" s="10"/>
-      <c r="X59" s="10"/>
-      <c r="Y59" s="10"/>
-      <c r="Z59" s="10"/>
+      <c r="A59" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C59" s="11"/>
+      <c r="D59" s="11"/>
+      <c r="E59" s="11"/>
+      <c r="F59" s="11"/>
+      <c r="G59" s="11"/>
+      <c r="H59" s="11"/>
+      <c r="I59" s="11"/>
+      <c r="J59" s="11"/>
+      <c r="K59" s="11"/>
+      <c r="L59" s="11"/>
+      <c r="M59" s="11"/>
+      <c r="N59" s="11"/>
+      <c r="O59" s="11"/>
+      <c r="P59" s="11"/>
+      <c r="Q59" s="11"/>
+      <c r="R59" s="11"/>
+      <c r="S59" s="11"/>
+      <c r="T59" s="11"/>
+      <c r="U59" s="11"/>
+      <c r="V59" s="11"/>
+      <c r="W59" s="11"/>
+      <c r="X59" s="11"/>
+      <c r="Y59" s="11"/>
+      <c r="Z59" s="11"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="B60" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="C60" s="10"/>
-      <c r="D60" s="10"/>
-      <c r="E60" s="10"/>
-      <c r="F60" s="10"/>
-      <c r="G60" s="10"/>
-      <c r="H60" s="10"/>
-      <c r="I60" s="10"/>
-      <c r="J60" s="10"/>
-      <c r="K60" s="10"/>
-      <c r="L60" s="10"/>
-      <c r="M60" s="10"/>
-      <c r="N60" s="10"/>
-      <c r="O60" s="10"/>
-      <c r="P60" s="10"/>
-      <c r="Q60" s="10"/>
-      <c r="R60" s="10"/>
-      <c r="S60" s="10"/>
-      <c r="T60" s="10"/>
-      <c r="U60" s="10"/>
-      <c r="V60" s="10"/>
-      <c r="W60" s="10"/>
-      <c r="X60" s="10"/>
-      <c r="Y60" s="10"/>
-      <c r="Z60" s="10"/>
+      <c r="A60" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C60" s="11"/>
+      <c r="D60" s="11"/>
+      <c r="E60" s="11"/>
+      <c r="F60" s="11"/>
+      <c r="G60" s="11"/>
+      <c r="H60" s="11"/>
+      <c r="I60" s="11"/>
+      <c r="J60" s="11"/>
+      <c r="K60" s="11"/>
+      <c r="L60" s="11"/>
+      <c r="M60" s="11"/>
+      <c r="N60" s="11"/>
+      <c r="O60" s="11"/>
+      <c r="P60" s="11"/>
+      <c r="Q60" s="11"/>
+      <c r="R60" s="11"/>
+      <c r="S60" s="11"/>
+      <c r="T60" s="11"/>
+      <c r="U60" s="11"/>
+      <c r="V60" s="11"/>
+      <c r="W60" s="11"/>
+      <c r="X60" s="11"/>
+      <c r="Y60" s="11"/>
+      <c r="Z60" s="11"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="A61" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="B61" s="7">
+      <c r="A61" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B61" s="8">
         <v>123456.0</v>
       </c>
-      <c r="C61" s="10"/>
-      <c r="D61" s="10"/>
-      <c r="E61" s="10"/>
-      <c r="F61" s="10"/>
-      <c r="G61" s="10"/>
-      <c r="H61" s="10"/>
-      <c r="I61" s="10"/>
-      <c r="J61" s="10"/>
-      <c r="K61" s="10"/>
-      <c r="L61" s="10"/>
-      <c r="M61" s="10"/>
-      <c r="N61" s="10"/>
-      <c r="O61" s="10"/>
-      <c r="P61" s="10"/>
-      <c r="Q61" s="10"/>
-      <c r="R61" s="10"/>
-      <c r="S61" s="10"/>
-      <c r="T61" s="10"/>
-      <c r="U61" s="10"/>
-      <c r="V61" s="10"/>
-      <c r="W61" s="10"/>
-      <c r="X61" s="10"/>
-      <c r="Y61" s="10"/>
-      <c r="Z61" s="10"/>
+      <c r="C61" s="11"/>
+      <c r="D61" s="11"/>
+      <c r="E61" s="11"/>
+      <c r="F61" s="11"/>
+      <c r="G61" s="11"/>
+      <c r="H61" s="11"/>
+      <c r="I61" s="11"/>
+      <c r="J61" s="11"/>
+      <c r="K61" s="11"/>
+      <c r="L61" s="11"/>
+      <c r="M61" s="11"/>
+      <c r="N61" s="11"/>
+      <c r="O61" s="11"/>
+      <c r="P61" s="11"/>
+      <c r="Q61" s="11"/>
+      <c r="R61" s="11"/>
+      <c r="S61" s="11"/>
+      <c r="T61" s="11"/>
+      <c r="U61" s="11"/>
+      <c r="V61" s="11"/>
+      <c r="W61" s="11"/>
+      <c r="X61" s="11"/>
+      <c r="Y61" s="11"/>
+      <c r="Z61" s="11"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="A62" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="B62" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="C62" s="10"/>
-      <c r="D62" s="10"/>
-      <c r="E62" s="10"/>
-      <c r="F62" s="10"/>
-      <c r="G62" s="10"/>
-      <c r="H62" s="10"/>
-      <c r="I62" s="10"/>
-      <c r="J62" s="10"/>
-      <c r="K62" s="10"/>
-      <c r="L62" s="10"/>
-      <c r="M62" s="10"/>
-      <c r="N62" s="10"/>
-      <c r="O62" s="10"/>
-      <c r="P62" s="10"/>
-      <c r="Q62" s="10"/>
-      <c r="R62" s="10"/>
-      <c r="S62" s="10"/>
-      <c r="T62" s="10"/>
-      <c r="U62" s="10"/>
-      <c r="V62" s="10"/>
-      <c r="W62" s="10"/>
-      <c r="X62" s="10"/>
-      <c r="Y62" s="10"/>
-      <c r="Z62" s="10"/>
+      <c r="A62" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C62" s="11"/>
+      <c r="D62" s="11"/>
+      <c r="E62" s="11"/>
+      <c r="F62" s="11"/>
+      <c r="G62" s="11"/>
+      <c r="H62" s="11"/>
+      <c r="I62" s="11"/>
+      <c r="J62" s="11"/>
+      <c r="K62" s="11"/>
+      <c r="L62" s="11"/>
+      <c r="M62" s="11"/>
+      <c r="N62" s="11"/>
+      <c r="O62" s="11"/>
+      <c r="P62" s="11"/>
+      <c r="Q62" s="11"/>
+      <c r="R62" s="11"/>
+      <c r="S62" s="11"/>
+      <c r="T62" s="11"/>
+      <c r="U62" s="11"/>
+      <c r="V62" s="11"/>
+      <c r="W62" s="11"/>
+      <c r="X62" s="11"/>
+      <c r="Y62" s="11"/>
+      <c r="Z62" s="11"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="A63" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="B63" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="C63" s="10"/>
-      <c r="D63" s="10"/>
-      <c r="E63" s="10"/>
-      <c r="F63" s="10"/>
-      <c r="G63" s="10"/>
-      <c r="H63" s="10"/>
-      <c r="I63" s="10"/>
-      <c r="J63" s="10"/>
-      <c r="K63" s="10"/>
-      <c r="L63" s="10"/>
-      <c r="M63" s="10"/>
-      <c r="N63" s="10"/>
-      <c r="O63" s="10"/>
-      <c r="P63" s="10"/>
-      <c r="Q63" s="10"/>
-      <c r="R63" s="10"/>
-      <c r="S63" s="10"/>
-      <c r="T63" s="10"/>
-      <c r="U63" s="10"/>
-      <c r="V63" s="10"/>
-      <c r="W63" s="10"/>
-      <c r="X63" s="10"/>
-      <c r="Y63" s="10"/>
-      <c r="Z63" s="10"/>
+      <c r="A63" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C63" s="11"/>
+      <c r="D63" s="11"/>
+      <c r="E63" s="11"/>
+      <c r="F63" s="11"/>
+      <c r="G63" s="11"/>
+      <c r="H63" s="11"/>
+      <c r="I63" s="11"/>
+      <c r="J63" s="11"/>
+      <c r="K63" s="11"/>
+      <c r="L63" s="11"/>
+      <c r="M63" s="11"/>
+      <c r="N63" s="11"/>
+      <c r="O63" s="11"/>
+      <c r="P63" s="11"/>
+      <c r="Q63" s="11"/>
+      <c r="R63" s="11"/>
+      <c r="S63" s="11"/>
+      <c r="T63" s="11"/>
+      <c r="U63" s="11"/>
+      <c r="V63" s="11"/>
+      <c r="W63" s="11"/>
+      <c r="X63" s="11"/>
+      <c r="Y63" s="11"/>
+      <c r="Z63" s="11"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="A64" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="B64" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="C64" s="10"/>
-      <c r="D64" s="10"/>
-      <c r="E64" s="10"/>
-      <c r="F64" s="10"/>
-      <c r="G64" s="10"/>
-      <c r="H64" s="10"/>
-      <c r="I64" s="10"/>
-      <c r="J64" s="10"/>
-      <c r="K64" s="10"/>
-      <c r="L64" s="10"/>
-      <c r="M64" s="10"/>
-      <c r="N64" s="10"/>
-      <c r="O64" s="10"/>
-      <c r="P64" s="10"/>
-      <c r="Q64" s="10"/>
-      <c r="R64" s="10"/>
-      <c r="S64" s="10"/>
-      <c r="T64" s="10"/>
-      <c r="U64" s="10"/>
-      <c r="V64" s="10"/>
-      <c r="W64" s="10"/>
-      <c r="X64" s="10"/>
-      <c r="Y64" s="10"/>
-      <c r="Z64" s="10"/>
+      <c r="A64" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="C64" s="11"/>
+      <c r="D64" s="11"/>
+      <c r="E64" s="11"/>
+      <c r="F64" s="11"/>
+      <c r="G64" s="11"/>
+      <c r="H64" s="11"/>
+      <c r="I64" s="11"/>
+      <c r="J64" s="11"/>
+      <c r="K64" s="11"/>
+      <c r="L64" s="11"/>
+      <c r="M64" s="11"/>
+      <c r="N64" s="11"/>
+      <c r="O64" s="11"/>
+      <c r="P64" s="11"/>
+      <c r="Q64" s="11"/>
+      <c r="R64" s="11"/>
+      <c r="S64" s="11"/>
+      <c r="T64" s="11"/>
+      <c r="U64" s="11"/>
+      <c r="V64" s="11"/>
+      <c r="W64" s="11"/>
+      <c r="X64" s="11"/>
+      <c r="Y64" s="11"/>
+      <c r="Z64" s="11"/>
     </row>
     <row r="65" ht="13.5" customHeight="1">
-      <c r="A65" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="B65" s="3"/>
-      <c r="C65" s="4"/>
-      <c r="D65" s="5"/>
-      <c r="E65" s="5"/>
-      <c r="F65" s="5"/>
-      <c r="G65" s="5"/>
-      <c r="H65" s="5"/>
-      <c r="I65" s="5"/>
-      <c r="J65" s="5"/>
-      <c r="K65" s="5"/>
-      <c r="L65" s="5"/>
-      <c r="M65" s="5"/>
-      <c r="N65" s="5"/>
-      <c r="O65" s="5"/>
+      <c r="A65" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="B65" s="4"/>
+      <c r="C65" s="5"/>
+      <c r="D65" s="6"/>
+      <c r="E65" s="6"/>
+      <c r="F65" s="6"/>
+      <c r="G65" s="6"/>
+      <c r="H65" s="6"/>
+      <c r="I65" s="6"/>
+      <c r="J65" s="6"/>
+      <c r="K65" s="6"/>
+      <c r="L65" s="6"/>
+      <c r="M65" s="6"/>
+      <c r="N65" s="6"/>
+      <c r="O65" s="6"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="A66" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="B66" s="7" t="s">
-        <v>124</v>
+      <c r="A66" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="A67" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="B67" s="7" t="s">
-        <v>126</v>
+      <c r="A67" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="A68" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="B68" s="7" t="s">
-        <v>128</v>
+      <c r="A68" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="69" ht="15.75" customHeight="1">
-      <c r="A69" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="B69" s="7" t="s">
-        <v>130</v>
+      <c r="A69" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="A70" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="B70" s="7" t="s">
-        <v>132</v>
+      <c r="A70" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="A71" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="B71" s="7" t="s">
+      <c r="A71" s="8" t="s">
         <v>134</v>
+      </c>
+      <c r="B71" s="8" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="72" ht="15.75" customHeight="1">
       <c r="A72" s="12" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B72" s="12" t="s">
         <v>137</v>
@@ -2189,179 +2171,179 @@
       <c r="A75" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="B75" s="6" t="s">
-        <v>83</v>
+      <c r="B75" s="7" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="76" ht="15.75" customHeight="1">
       <c r="A76" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="B76" s="7" t="s">
+      <c r="B76" s="8" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="77" ht="15.75" customHeight="1">
       <c r="A77" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="B77" s="8" t="s">
         <v>146</v>
-      </c>
-      <c r="B77" s="7" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="78" ht="15.75" customHeight="1">
       <c r="A78" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="B78" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="B78" s="7" t="s">
+    </row>
+    <row r="79" ht="15.75" customHeight="1">
+      <c r="A79" s="8" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="79" ht="15.75" customHeight="1">
-      <c r="A79" s="7" t="s">
+      <c r="B79" s="8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="80" ht="15.75" customHeight="1">
+      <c r="A80" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="B79" s="7" t="s">
+      <c r="B80" s="8" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="81" ht="15.75" customHeight="1">
+      <c r="A81" s="8" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="80" ht="15.75" customHeight="1">
-      <c r="A80" s="7" t="s">
+      <c r="B81" s="8" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="82" ht="15.75" customHeight="1">
+      <c r="A82" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="B82" s="13" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="83" ht="15.75" customHeight="1">
+      <c r="A83" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="B80" s="7" t="s">
+      <c r="B83" s="14" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="81" ht="15.75" customHeight="1">
-      <c r="A81" s="7" t="s">
+    <row r="84" ht="15.75" customHeight="1">
+      <c r="A84" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="B81" s="7" t="s">
+      <c r="B84" s="8" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="82" ht="15.75" customHeight="1">
-      <c r="A82" s="7" t="s">
+    <row r="85" ht="15.75" customHeight="1">
+      <c r="A85" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B85" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="B82" s="7" t="s">
+    </row>
+    <row r="86" ht="15.75" customHeight="1">
+      <c r="A86" s="8" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="83" ht="15.75" customHeight="1">
-      <c r="A83" s="7" t="s">
+      <c r="B86" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="B83" s="13" t="s">
+    </row>
+    <row r="87" ht="15.75" customHeight="1">
+      <c r="A87" s="8" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="84" ht="15.75" customHeight="1">
-      <c r="A84" s="7" t="s">
+      <c r="B87" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="B84" s="7" t="s">
+    </row>
+    <row r="88" ht="15.75" customHeight="1">
+      <c r="A88" s="8" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="85" ht="15.75" customHeight="1">
-      <c r="A85" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="B85" s="7" t="s">
+      <c r="B88" s="8" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="86" ht="15.75" customHeight="1">
-      <c r="A86" s="7" t="s">
+    <row r="89" ht="15.75" customHeight="1">
+      <c r="A89" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="B86" s="7" t="s">
+      <c r="B89" s="8" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="87" ht="15.75" customHeight="1">
-      <c r="A87" s="7" t="s">
+    <row r="90" ht="15.75" customHeight="1">
+      <c r="A90" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="B87" s="7" t="s">
+      <c r="B90" s="8" t="s">
         <v>168</v>
-      </c>
-    </row>
-    <row r="88" ht="15.75" customHeight="1">
-      <c r="A88" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="B88" s="7" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="89" ht="15.75" customHeight="1">
-      <c r="A89" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="B89" s="7" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="90" ht="15.75" customHeight="1">
-      <c r="A90" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="B90" s="7" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="91" ht="15.75" customHeight="1">
       <c r="A91" s="12" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B91" s="12" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
     </row>
     <row r="92" ht="15.75" customHeight="1">
       <c r="A92" s="12" t="s">
-        <v>177</v>
-      </c>
-      <c r="B92" s="7" t="s">
-        <v>178</v>
+        <v>171</v>
+      </c>
+      <c r="B92" s="8" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="93" ht="13.5" customHeight="1">
-      <c r="A93" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="B93" s="3"/>
-      <c r="C93" s="4"/>
-      <c r="D93" s="5"/>
-      <c r="E93" s="5"/>
-      <c r="F93" s="5"/>
-      <c r="G93" s="5"/>
-      <c r="H93" s="5"/>
-      <c r="I93" s="5"/>
-      <c r="J93" s="5"/>
-      <c r="K93" s="5"/>
-      <c r="L93" s="5"/>
-      <c r="M93" s="5"/>
-      <c r="N93" s="5"/>
-      <c r="O93" s="5"/>
+      <c r="A93" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="B93" s="4"/>
+      <c r="C93" s="5"/>
+      <c r="D93" s="6"/>
+      <c r="E93" s="6"/>
+      <c r="F93" s="6"/>
+      <c r="G93" s="6"/>
+      <c r="H93" s="6"/>
+      <c r="I93" s="6"/>
+      <c r="J93" s="6"/>
+      <c r="K93" s="6"/>
+      <c r="L93" s="6"/>
+      <c r="M93" s="6"/>
+      <c r="N93" s="6"/>
+      <c r="O93" s="6"/>
     </row>
     <row r="94" ht="15.75" customHeight="1">
-      <c r="A94" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B94" s="7" t="s">
-        <v>32</v>
+      <c r="A94" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B94" s="8" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="95" ht="15.75" customHeight="1">
-      <c r="A95" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B95" s="14" t="s">
-        <v>35</v>
+      <c r="A95" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B95" s="13" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="96" ht="15.75" customHeight="1"/>
@@ -3324,79 +3306,79 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
     </row>
     <row r="2">
-      <c r="A2" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
     </row>
     <row r="3">
-      <c r="A3" s="11" t="s">
-        <v>145</v>
-      </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
     </row>
     <row r="4">
-      <c r="A4" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
     </row>
     <row r="5">
-      <c r="A5" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
push latest test data file - naming convention
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/sendDashboard/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/sendDashboard/TestData.xlsx
@@ -14,12 +14,24 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="170">
   <si>
+    <t>Supported Browser Types</t>
+  </si>
+  <si>
+    <t>MozillaFirefox</t>
+  </si>
+  <si>
+    <t>GoogleChrome</t>
+  </si>
+  <si>
+    <t>MicrosoftInternetExplorer</t>
+  </si>
+  <si>
+    <t>MicrosoftEdge</t>
+  </si>
+  <si>
     <t>Variable</t>
   </si>
   <si>
-    <t>Supported Browser Types</t>
-  </si>
-  <si>
     <t>Data1</t>
   </si>
   <si>
@@ -32,18 +44,6 @@
     <t>Data4</t>
   </si>
   <si>
-    <t>MozillaFirefox</t>
-  </si>
-  <si>
-    <t>GoogleChrome</t>
-  </si>
-  <si>
-    <t>MicrosoftInternetExplorer</t>
-  </si>
-  <si>
-    <t>MicrosoftEdge</t>
-  </si>
-  <si>
     <t>URLs</t>
   </si>
   <si>
@@ -284,7 +284,7 @@
     <t>DashboardName</t>
   </si>
   <si>
-    <t>Sending Dashboard</t>
+    <t>Automation_Dashboard_SendDashboard</t>
   </si>
   <si>
     <t>HideNotificationToolTipText</t>
@@ -609,11 +609,11 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
@@ -721,20 +721,20 @@
   </cols>
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
@@ -3628,79 +3628,79 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>

</xml_diff>